<commit_message>
Board File Update on 9.18
</commit_message>
<xml_diff>
--- a/DeviceManagement/HIQC板卡统计及出借情况.xlsx
+++ b/DeviceManagement/HIQC板卡统计及出借情况.xlsx
@@ -1580,14 +1580,14 @@
       </c>
       <c r="R5" s="37">
         <f>=SUMIF($C$2:$C$200,"PYNQ-Z2",E2:E200)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S5" s="37">
         <v>21</v>
       </c>
       <c r="T5" s="37">
         <f>=S5-R5</f>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="U5" s="38" t="s"/>
     </row>
@@ -1840,14 +1840,14 @@
       </c>
       <c r="R9" s="45">
         <f>=SUMIF($C$2:$C$200,"ACX750",E2:E200)</f>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S9" s="45">
         <v>40</v>
       </c>
       <c r="T9" s="45">
         <f>=S9-R9</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="U9" s="36" t="s"/>
     </row>
@@ -2724,11 +2724,11 @@
         <v>53</v>
       </c>
       <c r="D25" s="13">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E25" s="13">
         <f>=D25-O25</f>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F25" s="13" t="s">
         <v>72</v>
@@ -2864,16 +2864,22 @@
       <c r="A28" s="13">
         <v>26</v>
       </c>
-      <c r="B28" s="10" t="s"/>
-      <c r="C28" s="28" t="s"/>
+      <c r="B28" s="76">
+        <v>45918</v>
+      </c>
+      <c r="C28" s="28" t="s">
+        <v>26</v>
+      </c>
       <c r="D28" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28" s="13">
         <f>=D28-O28</f>
-        <v>0</v>
-      </c>
-      <c r="F28" s="13" t="s"/>
+        <v>1</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>72</v>
+      </c>
       <c r="G28" s="10" t="s"/>
       <c r="H28" s="28" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Board File Update on 9.23
</commit_message>
<xml_diff>
--- a/DeviceManagement/HIQC板卡统计及出借情况.xlsx
+++ b/DeviceManagement/HIQC板卡统计及出借情况.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t/>
   </si>
@@ -236,6 +236,9 @@
   </si>
   <si>
     <t>PLD竞赛</t>
+  </si>
+  <si>
+    <t>李雨龙</t>
   </si>
   <si>
     <r>
@@ -1414,7 +1417,7 @@
         <v>1</v>
       </c>
       <c r="P2" s="23" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="Q2" s="24" t="s"/>
       <c r="R2" s="25" t="s"/>
@@ -1931,14 +1934,14 @@
       </c>
       <c r="R10" s="48">
         <f>=SUMIF($C$2:$C$200,"MLK-KU060",E2:E200)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S10" s="48">
         <v>13</v>
       </c>
       <c r="T10" s="48">
         <f>=S10-R10</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="U10" s="38" t="s"/>
     </row>
@@ -1990,7 +1993,7 @@
         <v>8</v>
       </c>
       <c r="Q11" s="50" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="R11" s="51">
         <f>=SUMIF($C$2:$C$200,"VD100",E2:E200)</f>
@@ -2472,7 +2475,7 @@
         <v>21</v>
       </c>
       <c r="I19" s="29" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="J19" s="29" t="s">
         <v>45</v>
@@ -2532,7 +2535,7 @@
         <v>21</v>
       </c>
       <c r="I20" s="29" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="J20" s="29" t="s">
         <v>45</v>
@@ -2779,7 +2782,7 @@
         <v>21</v>
       </c>
       <c r="I25" s="29" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="J25" s="29" t="s">
         <v>45</v>
@@ -2828,7 +2831,7 @@
         <v>21</v>
       </c>
       <c r="I26" s="29" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="J26" s="29" t="s">
         <v>45</v>
@@ -2877,7 +2880,7 @@
         <v>21</v>
       </c>
       <c r="I27" s="29" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="J27" s="29" t="s">
         <v>45</v>
@@ -2926,7 +2929,7 @@
         <v>21</v>
       </c>
       <c r="I28" s="29" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="J28" s="29" t="s">
         <v>45</v>
@@ -2953,16 +2956,22 @@
       <c r="A29" s="14">
         <v>27</v>
       </c>
-      <c r="B29" s="10" t="s"/>
-      <c r="C29" s="29" t="s"/>
+      <c r="B29" s="84">
+        <v>45923</v>
+      </c>
+      <c r="C29" s="29" t="s">
+        <v>44</v>
+      </c>
       <c r="D29" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29" s="14">
         <f>=D29-O29</f>
-        <v>0</v>
-      </c>
-      <c r="F29" s="14" t="s"/>
+        <v>1</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>74</v>
+      </c>
       <c r="G29" s="10" t="s"/>
       <c r="H29" s="29" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Board File Update on 10.9
</commit_message>
<xml_diff>
--- a/DeviceManagement/HIQC板卡统计及出借情况.xlsx
+++ b/DeviceManagement/HIQC板卡统计及出借情况.xlsx
@@ -1611,14 +1611,14 @@
       </c>
       <c r="R5" s="39">
         <f>=SUMIF($C$2:$C$200,"PYNQ-Z2",E2:E200)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S5" s="39">
         <v>21</v>
       </c>
       <c r="T5" s="39">
         <f>=S5-R5</f>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="U5" s="40" t="s"/>
     </row>
@@ -1871,14 +1871,14 @@
       </c>
       <c r="R9" s="47">
         <f>=SUMIF($C$2:$C$200,"ACX750",E2:E200)</f>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="S9" s="47">
         <v>40</v>
       </c>
       <c r="T9" s="47">
         <f>=S9-R9</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="U9" s="38" t="s"/>
     </row>
@@ -2768,11 +2768,11 @@
         <v>53</v>
       </c>
       <c r="D25" s="14">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E25" s="14">
         <f>=D25-O25</f>
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F25" s="14" t="s">
         <v>73</v>
@@ -3004,16 +3004,22 @@
       <c r="A30" s="14">
         <v>28</v>
       </c>
-      <c r="B30" s="10" t="s"/>
-      <c r="C30" s="29" t="s"/>
+      <c r="B30" s="84">
+        <v>45939</v>
+      </c>
+      <c r="C30" s="29" t="s">
+        <v>26</v>
+      </c>
       <c r="D30" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30" s="14">
         <f>=D30-O30</f>
-        <v>0</v>
-      </c>
-      <c r="F30" s="14" t="s"/>
+        <v>1</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>73</v>
+      </c>
       <c r="G30" s="10" t="s"/>
       <c r="H30" s="29" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Board File Update on 10.11
</commit_message>
<xml_diff>
--- a/DeviceManagement/HIQC板卡统计及出借情况.xlsx
+++ b/DeviceManagement/HIQC板卡统计及出借情况.xlsx
@@ -1871,14 +1871,14 @@
       </c>
       <c r="R9" s="47">
         <f>=SUMIF($C$2:$C$200,"ACX750",E2:E200)</f>
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="S9" s="47">
         <v>40</v>
       </c>
       <c r="T9" s="47">
         <f>=S9-R9</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="U9" s="38" t="s"/>
     </row>
@@ -2190,14 +2190,14 @@
       </c>
       <c r="R14" s="61">
         <f>=SUMIF($C$2:$C$200,"KV260",E2:E200)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S14" s="61">
         <v>4</v>
       </c>
       <c r="T14" s="62">
         <f>=S14-R14</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U14" s="63" t="s"/>
     </row>
@@ -2768,11 +2768,11 @@
         <v>53</v>
       </c>
       <c r="D25" s="14">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E25" s="14">
         <f>=D25-O25</f>
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F25" s="14" t="s">
         <v>73</v>
@@ -3052,16 +3052,22 @@
       <c r="A31" s="14">
         <v>29</v>
       </c>
-      <c r="B31" s="10" t="s"/>
-      <c r="C31" s="29" t="s"/>
+      <c r="B31" s="84">
+        <v>45941</v>
+      </c>
+      <c r="C31" s="29" t="s">
+        <v>51</v>
+      </c>
       <c r="D31" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E31" s="14">
         <f>=D31-O31</f>
-        <v>0</v>
-      </c>
-      <c r="F31" s="14" t="s"/>
+        <v>1</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>73</v>
+      </c>
       <c r="G31" s="10" t="s"/>
       <c r="H31" s="29" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Board File Update on 10.15
</commit_message>
<xml_diff>
--- a/DeviceManagement/HIQC板卡统计及出借情况.xlsx
+++ b/DeviceManagement/HIQC板卡统计及出借情况.xlsx
@@ -2062,14 +2062,14 @@
       </c>
       <c r="R12" s="55">
         <f>=SUMIF($C$2:$C$200,"Alveo-U45N",E2:E200)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S12" s="56">
         <v>2</v>
       </c>
       <c r="T12" s="57">
         <f>=S12-R12</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U12" s="58" t="s"/>
     </row>
@@ -2670,7 +2670,7 @@
       </c>
       <c r="E23" s="14">
         <f>=D23-O23</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23" s="14" t="s">
         <v>39</v>
@@ -2690,14 +2690,14 @@
       <c r="K23" s="11" t="s"/>
       <c r="L23" s="21" t="s"/>
       <c r="M23" s="31" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="N23" s="21">
         <v>0</v>
       </c>
       <c r="O23" s="14">
         <f>=IF(M23="是",D23-N23,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q23" s="81" t="s"/>
       <c r="R23" s="81" t="s"/>

</xml_diff>

<commit_message>
Board File Update on 10.24
</commit_message>
<xml_diff>
--- a/DeviceManagement/HIQC板卡统计及出借情况.xlsx
+++ b/DeviceManagement/HIQC板卡统计及出借情况.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <si>
     <t/>
   </si>
@@ -239,6 +239,9 @@
   </si>
   <si>
     <t>李雨龙</t>
+  </si>
+  <si>
+    <t>研究生课程</t>
   </si>
   <si>
     <r>
@@ -1417,7 +1420,7 @@
         <v>1</v>
       </c>
       <c r="P2" s="23" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="Q2" s="24" t="s"/>
       <c r="R2" s="25" t="s"/>
@@ -1611,14 +1614,14 @@
       </c>
       <c r="R5" s="39">
         <f>=SUMIF($C$2:$C$200,"PYNQ-Z2",E2:E200)</f>
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="S5" s="39">
         <v>21</v>
       </c>
       <c r="T5" s="39">
         <f>=S5-R5</f>
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="U5" s="40" t="s"/>
     </row>
@@ -1871,14 +1874,14 @@
       </c>
       <c r="R9" s="47">
         <f>=SUMIF($C$2:$C$200,"ACX750",E2:E200)</f>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="S9" s="47">
         <v>40</v>
       </c>
       <c r="T9" s="47">
         <f>=S9-R9</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="U9" s="38" t="s"/>
     </row>
@@ -1993,7 +1996,7 @@
         <v>8</v>
       </c>
       <c r="Q11" s="50" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="R11" s="51">
         <f>=SUMIF($C$2:$C$200,"VD100",E2:E200)</f>
@@ -2768,11 +2771,11 @@
         <v>53</v>
       </c>
       <c r="D25" s="14">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E25" s="14">
         <f>=D25-O25</f>
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F25" s="14" t="s">
         <v>73</v>
@@ -2919,7 +2922,7 @@
       </c>
       <c r="E28" s="14">
         <f>=D28-O28</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F28" s="14" t="s">
         <v>73</v>
@@ -2937,14 +2940,14 @@
       <c r="K28" s="11" t="s"/>
       <c r="L28" s="21" t="s"/>
       <c r="M28" s="31" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="N28" s="21">
         <v>0</v>
       </c>
       <c r="O28" s="14">
         <f>=IF(M28="是",D28-N28,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q28" s="81" t="s"/>
       <c r="S28" s="86" t="s"/>
@@ -3011,11 +3014,11 @@
         <v>26</v>
       </c>
       <c r="D30" s="14">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E30" s="14">
         <f>=D30-O30</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F30" s="14" t="s">
         <v>73</v>
@@ -3025,7 +3028,7 @@
         <v>21</v>
       </c>
       <c r="I30" s="29" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="J30" s="29" t="s">
         <v>45</v>
@@ -3073,7 +3076,7 @@
         <v>21</v>
       </c>
       <c r="I31" s="29" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="J31" s="29" t="s">
         <v>45</v>
@@ -3101,22 +3104,28 @@
       <c r="A32" s="14">
         <v>30</v>
       </c>
-      <c r="B32" s="10" t="s"/>
-      <c r="C32" s="29" t="s"/>
+      <c r="B32" s="84">
+        <v>45954</v>
+      </c>
+      <c r="C32" s="29" t="s">
+        <v>26</v>
+      </c>
       <c r="D32" s="14">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E32" s="14">
         <f>=D32-O32</f>
-        <v>0</v>
-      </c>
-      <c r="F32" s="14" t="s"/>
+        <v>9</v>
+      </c>
+      <c r="F32" s="14" t="s">
+        <v>75</v>
+      </c>
       <c r="G32" s="10" t="s"/>
       <c r="H32" s="29" t="s">
         <v>21</v>
       </c>
       <c r="I32" s="29" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="J32" s="29" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
Board File Update on 10.27
</commit_message>
<xml_diff>
--- a/DeviceManagement/HIQC板卡统计及出借情况.xlsx
+++ b/DeviceManagement/HIQC板卡统计及出借情况.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
   <si>
     <t/>
   </si>
@@ -226,6 +226,9 @@
     <t>Boolean</t>
   </si>
   <si>
+    <t>ZU19EG</t>
+  </si>
+  <si>
     <t>AXP391</t>
   </si>
   <si>
@@ -242,6 +245,9 @@
   </si>
   <si>
     <t>研究生课程</t>
+  </si>
+  <si>
+    <t>陈凯</t>
   </si>
   <si>
     <r>
@@ -329,7 +335,7 @@
     <numFmt numFmtId="300" formatCode="yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;;@"/>
     <numFmt numFmtId="301" formatCode="yyyy&quot;年&quot;m&quot;月&quot;;@"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="19">
     <font>
       <name val="等线"/>
       <charset val="134"/>
@@ -393,13 +399,10 @@
     </font>
     <font/>
     <font/>
-    <font>
-      <color rgb="FF000000"/>
-    </font>
     <font/>
     <font/>
   </fonts>
-  <fills count="30">
+  <fills count="31">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -525,6 +528,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFBFBFBF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE5EFFF"/>
       </patternFill>
     </fill>
     <fill/>
@@ -681,7 +689,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -925,31 +933,40 @@
     <xf fontId="12" fillId="26" borderId="1" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="12" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="1" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="12" fillId="27" borderId="12" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="13" fillId="27" borderId="1" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="17" fillId="3" borderId="5" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="300" fontId="0" fillId="0" borderId="1" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf fontId="9" fillId="3" borderId="5" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf fontId="17" fillId="3" borderId="5" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf fontId="18" fillId="3" borderId="5" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="300" fontId="0" fillId="0" borderId="1" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf fontId="5" fillId="27" borderId="5" xfId="0">
+    <xf fontId="5" fillId="28" borderId="5" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf fontId="9" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="27" borderId="10" xfId="0">
+    <xf fontId="0" fillId="28" borderId="10" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf fontId="9" fillId="3" borderId="13" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf fontId="9" fillId="27" borderId="13" xfId="0">
+    <xf fontId="9" fillId="28" borderId="13" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf fontId="5" fillId="0" borderId="5" xfId="0">
@@ -973,7 +990,7 @@
     <xf fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf fontId="19" fillId="28" borderId="15" xfId="0">
+    <xf fontId="18" fillId="29" borderId="15" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf fontId="3" fillId="0" borderId="0" xfId="0">
@@ -982,7 +999,7 @@
     <xf fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="29" borderId="0" xfId="0">
+    <xf fontId="0" fillId="30" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1299,17 +1316,17 @@
     <col min="2" max="2" width="15.7812" customWidth="true"/>
     <col min="4" max="4" width="10.3828" customWidth="true"/>
     <col min="5" max="5" width="9.71094" hidden="true" customWidth="true"/>
-    <col min="6" max="6" width="13.6719" style="99"/>
+    <col min="6" max="6" width="13.6719" style="102"/>
     <col min="9" max="10" width="9.30078" customWidth="true"/>
     <col min="11" max="11" width="15.6406" customWidth="true"/>
     <col min="13" max="13" width="9.44141" style="14" customWidth="true"/>
     <col min="14" max="14" width="9.17188" style="14" customWidth="true"/>
     <col min="15" max="15" width="10.6523" style="14" customWidth="true"/>
-    <col min="17" max="17" width="21.582" style="86" customWidth="true"/>
-    <col min="18" max="18" width="17.2617" style="86" customWidth="true"/>
-    <col min="19" max="19" width="18.4844" style="92" customWidth="true"/>
-    <col min="20" max="20" width="9.57422" style="92" customWidth="true"/>
-    <col min="21" max="21" width="16.3242" style="100" customWidth="true"/>
+    <col min="17" max="17" width="21.582" style="89" customWidth="true"/>
+    <col min="18" max="18" width="17.2617" style="89" customWidth="true"/>
+    <col min="19" max="19" width="18.4844" style="95" customWidth="true"/>
+    <col min="20" max="20" width="9.57422" style="95" customWidth="true"/>
+    <col min="21" max="21" width="16.3242" style="103" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="27.75" customHeight="true">
@@ -1420,7 +1437,7 @@
         <v>1</v>
       </c>
       <c r="P2" s="23" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="Q2" s="24" t="s"/>
       <c r="R2" s="25" t="s"/>
@@ -1996,7 +2013,7 @@
         <v>8</v>
       </c>
       <c r="Q11" s="50" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="R11" s="51">
         <f>=SUMIF($C$2:$C$200,"VD100",E2:E200)</f>
@@ -2555,22 +2572,35 @@
         <f>=IF(M20="是",D20-N20,0)</f>
         <v>6</v>
       </c>
-      <c r="Q20" s="81" t="s"/>
-      <c r="R20" s="81" t="s"/>
-      <c r="S20" s="81" t="s"/>
-      <c r="T20" s="82" t="s"/>
-      <c r="U20" s="83" t="s"/>
+      <c r="P20" s="49">
+        <v>17</v>
+      </c>
+      <c r="Q20" s="81" t="s">
+        <v>70</v>
+      </c>
+      <c r="R20" s="82">
+        <f>=SUMIF($C$2:$C$200,"ZU19EG",E2:E200)</f>
+        <v>1</v>
+      </c>
+      <c r="S20" s="83">
+        <v>1</v>
+      </c>
+      <c r="T20" s="84">
+        <f>=S20-R20</f>
+        <v>0</v>
+      </c>
+      <c r="U20" s="85" t="s"/>
       <c r="V20" s="54" t="s"/>
     </row>
     <row r="21" spans="1:22">
       <c r="A21" s="14">
         <v>19</v>
       </c>
-      <c r="B21" s="84">
+      <c r="B21" s="86">
         <v>45901</v>
       </c>
       <c r="C21" s="29" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D21" s="14">
         <v>1</v>
@@ -2580,7 +2610,7 @@
         <v>0</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G21" s="10" t="s"/>
       <c r="H21" s="29" t="s">
@@ -2604,18 +2634,18 @@
         <f>=IF(M21="是",D21-N21,0)</f>
         <v>1</v>
       </c>
-      <c r="Q21" s="81" t="s"/>
-      <c r="R21" s="81" t="s"/>
-      <c r="S21" s="81" t="s"/>
-      <c r="T21" s="81" t="s"/>
-      <c r="U21" s="85" t="s"/>
+      <c r="Q21" s="87" t="s"/>
+      <c r="R21" s="87" t="s"/>
+      <c r="S21" s="87" t="s"/>
+      <c r="T21" s="87" t="s"/>
+      <c r="U21" s="88" t="s"/>
       <c r="V21" s="54" t="s"/>
     </row>
     <row r="22" spans="1:22">
       <c r="A22" s="14">
         <v>20</v>
       </c>
-      <c r="B22" s="84">
+      <c r="B22" s="86">
         <v>45903</v>
       </c>
       <c r="C22" s="29" t="s">
@@ -2629,7 +2659,7 @@
         <v>2</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G22" s="10" t="s"/>
       <c r="H22" s="29" t="s">
@@ -2653,11 +2683,11 @@
         <f>=IF(M22="是",D22-N22,0)</f>
         <v>0</v>
       </c>
-      <c r="Q22" s="81" t="s"/>
-      <c r="R22" s="81" t="s"/>
-      <c r="S22" s="81" t="s"/>
-      <c r="T22" s="81" t="s"/>
-      <c r="U22" s="85" t="s"/>
+      <c r="Q22" s="87" t="s"/>
+      <c r="R22" s="87" t="s"/>
+      <c r="S22" s="87" t="s"/>
+      <c r="T22" s="87" t="s"/>
+      <c r="U22" s="88" t="s"/>
       <c r="V22" s="54" t="s"/>
     </row>
     <row r="23" spans="1:22">
@@ -2702,22 +2732,22 @@
         <f>=IF(M23="是",D23-N23,0)</f>
         <v>1</v>
       </c>
-      <c r="Q23" s="81" t="s"/>
-      <c r="R23" s="81" t="s"/>
-      <c r="S23" s="81" t="s"/>
-      <c r="T23" s="81" t="s"/>
-      <c r="U23" s="85" t="s"/>
+      <c r="Q23" s="87" t="s"/>
+      <c r="R23" s="87" t="s"/>
+      <c r="S23" s="87" t="s"/>
+      <c r="T23" s="87" t="s"/>
+      <c r="U23" s="88" t="s"/>
       <c r="V23" s="54" t="s"/>
     </row>
     <row r="24" spans="1:22">
       <c r="A24" s="14">
         <v>22</v>
       </c>
-      <c r="B24" s="84">
+      <c r="B24" s="86">
         <v>45912</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D24" s="14">
         <v>1</v>
@@ -2753,18 +2783,18 @@
         <f>=IF(M24="是",D24-N24,0)</f>
         <v>0</v>
       </c>
-      <c r="Q24" s="81" t="s"/>
-      <c r="R24" s="81" t="s"/>
-      <c r="S24" s="81" t="s"/>
-      <c r="T24" s="81" t="s"/>
-      <c r="U24" s="85" t="s"/>
+      <c r="Q24" s="87" t="s"/>
+      <c r="R24" s="87" t="s"/>
+      <c r="S24" s="87" t="s"/>
+      <c r="T24" s="87" t="s"/>
+      <c r="U24" s="88" t="s"/>
       <c r="V24" s="54" t="s"/>
     </row>
     <row r="25" spans="1:22">
       <c r="A25" s="14">
         <v>23</v>
       </c>
-      <c r="B25" s="84">
+      <c r="B25" s="86">
         <v>45917</v>
       </c>
       <c r="C25" s="29" t="s">
@@ -2778,7 +2808,7 @@
         <v>29</v>
       </c>
       <c r="F25" s="14" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G25" s="10" t="s"/>
       <c r="H25" s="29" t="s">
@@ -2802,18 +2832,18 @@
         <f>=IF(M25="是",D25-N25,0)</f>
         <v>0</v>
       </c>
-      <c r="Q25" s="81" t="s"/>
-      <c r="R25" s="81" t="s"/>
-      <c r="S25" s="81" t="s"/>
-      <c r="T25" s="81" t="s"/>
-      <c r="U25" s="85" t="s"/>
+      <c r="Q25" s="87" t="s"/>
+      <c r="R25" s="87" t="s"/>
+      <c r="S25" s="87" t="s"/>
+      <c r="T25" s="87" t="s"/>
+      <c r="U25" s="88" t="s"/>
       <c r="V25" s="54" t="s"/>
     </row>
     <row r="26" spans="1:22">
       <c r="A26" s="14">
         <v>24</v>
       </c>
-      <c r="B26" s="84">
+      <c r="B26" s="86">
         <v>45917</v>
       </c>
       <c r="C26" s="29" t="s">
@@ -2827,7 +2857,7 @@
         <v>40</v>
       </c>
       <c r="F26" s="14" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G26" s="10" t="s"/>
       <c r="H26" s="29" t="s">
@@ -2851,18 +2881,18 @@
         <f>=IF(M26="是",D26-N26,0)</f>
         <v>0</v>
       </c>
-      <c r="Q26" s="81" t="s"/>
-      <c r="R26" s="81" t="s"/>
-      <c r="S26" s="81" t="s"/>
-      <c r="T26" s="81" t="s"/>
-      <c r="U26" s="85" t="s"/>
+      <c r="Q26" s="87" t="s"/>
+      <c r="R26" s="87" t="s"/>
+      <c r="S26" s="87" t="s"/>
+      <c r="T26" s="87" t="s"/>
+      <c r="U26" s="88" t="s"/>
       <c r="V26" s="54" t="s"/>
     </row>
     <row r="27" spans="1:22">
       <c r="A27" s="14">
         <v>25</v>
       </c>
-      <c r="B27" s="84">
+      <c r="B27" s="86">
         <v>45917</v>
       </c>
       <c r="C27" s="29" t="s">
@@ -2876,7 +2906,7 @@
         <v>1</v>
       </c>
       <c r="F27" s="14" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G27" s="10" t="s"/>
       <c r="H27" s="29" t="s">
@@ -2900,18 +2930,18 @@
         <f>=IF(M27="是",D27-N27,0)</f>
         <v>0</v>
       </c>
-      <c r="Q27" s="81" t="s"/>
-      <c r="R27" s="81" t="s"/>
-      <c r="S27" s="81" t="s"/>
-      <c r="T27" s="81" t="s"/>
-      <c r="U27" s="85" t="s"/>
+      <c r="Q27" s="87" t="s"/>
+      <c r="R27" s="87" t="s"/>
+      <c r="S27" s="87" t="s"/>
+      <c r="T27" s="87" t="s"/>
+      <c r="U27" s="88" t="s"/>
       <c r="V27" s="54" t="s"/>
     </row>
     <row r="28" spans="1:22">
       <c r="A28" s="14">
         <v>26</v>
       </c>
-      <c r="B28" s="84">
+      <c r="B28" s="86">
         <v>45918</v>
       </c>
       <c r="C28" s="29" t="s">
@@ -2925,7 +2955,7 @@
         <v>0</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G28" s="10" t="s"/>
       <c r="H28" s="29" t="s">
@@ -2949,17 +2979,17 @@
         <f>=IF(M28="是",D28-N28,0)</f>
         <v>1</v>
       </c>
-      <c r="Q28" s="81" t="s"/>
-      <c r="S28" s="86" t="s"/>
-      <c r="T28" s="86" t="s"/>
+      <c r="Q28" s="87" t="s"/>
+      <c r="S28" s="89" t="s"/>
+      <c r="T28" s="89" t="s"/>
       <c r="U28" s="35" t="s"/>
-      <c r="V28" s="87" t="s"/>
+      <c r="V28" s="90" t="s"/>
     </row>
     <row r="29" spans="1:22">
       <c r="A29" s="14">
         <v>27</v>
       </c>
-      <c r="B29" s="84">
+      <c r="B29" s="86">
         <v>45923</v>
       </c>
       <c r="C29" s="29" t="s">
@@ -2973,7 +3003,7 @@
         <v>1</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G29" s="10" t="s"/>
       <c r="H29" s="29" t="s">
@@ -2997,17 +3027,17 @@
         <f>=IF(M29="是",D29-N29,0)</f>
         <v>0</v>
       </c>
-      <c r="Q29" s="81" t="s"/>
-      <c r="S29" s="86" t="s"/>
-      <c r="T29" s="86" t="s"/>
+      <c r="Q29" s="87" t="s"/>
+      <c r="S29" s="89" t="s"/>
+      <c r="T29" s="89" t="s"/>
       <c r="U29" s="35" t="s"/>
-      <c r="V29" s="87" t="s"/>
+      <c r="V29" s="90" t="s"/>
     </row>
     <row r="30" spans="1:22">
       <c r="A30" s="14">
         <v>28</v>
       </c>
-      <c r="B30" s="84">
+      <c r="B30" s="86">
         <v>45939</v>
       </c>
       <c r="C30" s="29" t="s">
@@ -3021,7 +3051,7 @@
         <v>4</v>
       </c>
       <c r="F30" s="14" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G30" s="10" t="s"/>
       <c r="H30" s="29" t="s">
@@ -3045,17 +3075,17 @@
         <f>=IF(M30="是",D30-N30,0)</f>
         <v>0</v>
       </c>
-      <c r="Q30" s="81" t="s"/>
-      <c r="S30" s="86" t="s"/>
-      <c r="T30" s="86" t="s"/>
+      <c r="Q30" s="87" t="s"/>
+      <c r="S30" s="89" t="s"/>
+      <c r="T30" s="89" t="s"/>
       <c r="U30" s="35" t="s"/>
-      <c r="V30" s="87" t="s"/>
+      <c r="V30" s="90" t="s"/>
     </row>
     <row r="31" spans="1:22">
       <c r="A31" s="14">
         <v>29</v>
       </c>
-      <c r="B31" s="84">
+      <c r="B31" s="86">
         <v>45941</v>
       </c>
       <c r="C31" s="29" t="s">
@@ -3069,7 +3099,7 @@
         <v>1</v>
       </c>
       <c r="F31" s="14" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G31" s="10" t="s"/>
       <c r="H31" s="29" t="s">
@@ -3093,18 +3123,18 @@
         <f>=IF(M31="是",D31-N31,0)</f>
         <v>0</v>
       </c>
-      <c r="Q31" s="88" t="s"/>
-      <c r="R31" s="89" t="s"/>
-      <c r="S31" s="90" t="s"/>
-      <c r="T31" s="86" t="s"/>
-      <c r="U31" s="91" t="s"/>
-      <c r="V31" s="87" t="s"/>
+      <c r="Q31" s="91" t="s"/>
+      <c r="R31" s="92" t="s"/>
+      <c r="S31" s="93" t="s"/>
+      <c r="T31" s="89" t="s"/>
+      <c r="U31" s="94" t="s"/>
+      <c r="V31" s="90" t="s"/>
     </row>
     <row r="32" spans="1:22">
       <c r="A32" s="14">
         <v>30</v>
       </c>
-      <c r="B32" s="84">
+      <c r="B32" s="86">
         <v>45954</v>
       </c>
       <c r="C32" s="29" t="s">
@@ -3118,7 +3148,7 @@
         <v>9</v>
       </c>
       <c r="F32" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G32" s="10" t="s"/>
       <c r="H32" s="29" t="s">
@@ -3142,27 +3172,33 @@
         <f>=IF(M32="是",D32-N32,0)</f>
         <v>0</v>
       </c>
-      <c r="Q32" s="88" t="s"/>
-      <c r="R32" s="89" t="s"/>
-      <c r="S32" s="90" t="s"/>
-      <c r="T32" s="86" t="s"/>
-      <c r="U32" s="91" t="s"/>
-      <c r="V32" s="87" t="s"/>
+      <c r="Q32" s="91" t="s"/>
+      <c r="R32" s="92" t="s"/>
+      <c r="S32" s="93" t="s"/>
+      <c r="T32" s="89" t="s"/>
+      <c r="U32" s="94" t="s"/>
+      <c r="V32" s="90" t="s"/>
     </row>
     <row r="33" spans="1:21">
       <c r="A33" s="14">
         <v>31</v>
       </c>
-      <c r="B33" s="10" t="s"/>
-      <c r="C33" s="29" t="s"/>
+      <c r="B33" s="86">
+        <v>45957</v>
+      </c>
+      <c r="C33" s="29" t="s">
+        <v>70</v>
+      </c>
       <c r="D33" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E33" s="14">
         <f>=D33-O33</f>
-        <v>0</v>
-      </c>
-      <c r="F33" s="14" t="s"/>
+        <v>1</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>77</v>
+      </c>
       <c r="G33" s="10" t="s"/>
       <c r="H33" s="29" t="s">
         <v>21</v>
@@ -3185,11 +3221,11 @@
         <f>=IF(M33="是",D33-N33,0)</f>
         <v>0</v>
       </c>
-      <c r="Q33" s="88" t="s"/>
-      <c r="R33" s="89" t="s"/>
-      <c r="S33" s="90" t="s"/>
-      <c r="T33" s="86" t="s"/>
-      <c r="U33" s="91" t="s"/>
+      <c r="Q33" s="91" t="s"/>
+      <c r="R33" s="92" t="s"/>
+      <c r="S33" s="93" t="s"/>
+      <c r="T33" s="89" t="s"/>
+      <c r="U33" s="94" t="s"/>
     </row>
     <row r="34" spans="1:21">
       <c r="A34" s="14">
@@ -3227,9 +3263,9 @@
         <f>=IF(M34="是",D34-N34,0)</f>
         <v>0</v>
       </c>
-      <c r="Q34" s="81" t="s"/>
-      <c r="S34" s="86" t="s"/>
-      <c r="T34" s="86" t="s"/>
+      <c r="Q34" s="87" t="s"/>
+      <c r="S34" s="89" t="s"/>
+      <c r="T34" s="89" t="s"/>
       <c r="U34" s="35" t="s"/>
     </row>
     <row r="35" spans="1:22">
@@ -3268,11 +3304,11 @@
         <f>=IF(M35="是",D35-N35,0)</f>
         <v>0</v>
       </c>
-      <c r="Q35" s="81" t="s"/>
-      <c r="S35" s="86" t="s"/>
-      <c r="T35" s="86" t="s"/>
+      <c r="Q35" s="87" t="s"/>
+      <c r="S35" s="89" t="s"/>
+      <c r="T35" s="89" t="s"/>
       <c r="U35" s="35" t="s"/>
-      <c r="V35" s="87" t="s"/>
+      <c r="V35" s="90" t="s"/>
     </row>
     <row r="36" spans="1:22">
       <c r="A36" s="14">
@@ -3310,11 +3346,11 @@
         <f>=IF(M36="是",D36-N36,0)</f>
         <v>0</v>
       </c>
-      <c r="Q36" s="81" t="s"/>
-      <c r="S36" s="86" t="s"/>
-      <c r="T36" s="86" t="s"/>
+      <c r="Q36" s="87" t="s"/>
+      <c r="S36" s="89" t="s"/>
+      <c r="T36" s="89" t="s"/>
       <c r="U36" s="35" t="s"/>
-      <c r="V36" s="87" t="s"/>
+      <c r="V36" s="90" t="s"/>
     </row>
     <row r="37" spans="1:22">
       <c r="A37" s="14">
@@ -3352,11 +3388,11 @@
         <f>=IF(M37="是",D37-N37,0)</f>
         <v>0</v>
       </c>
-      <c r="Q37" s="81" t="s"/>
-      <c r="S37" s="86" t="s"/>
-      <c r="T37" s="86" t="s"/>
+      <c r="Q37" s="87" t="s"/>
+      <c r="S37" s="89" t="s"/>
+      <c r="T37" s="89" t="s"/>
       <c r="U37" s="35" t="s"/>
-      <c r="V37" s="87" t="s"/>
+      <c r="V37" s="90" t="s"/>
     </row>
     <row r="38" spans="1:21">
       <c r="A38" s="14">
@@ -3394,8 +3430,8 @@
         <f>=IF(M38="是",D38-N38,0)</f>
         <v>0</v>
       </c>
-      <c r="S38" s="86" t="s"/>
-      <c r="T38" s="86" t="s"/>
+      <c r="S38" s="89" t="s"/>
+      <c r="T38" s="89" t="s"/>
       <c r="U38" s="35" t="s"/>
     </row>
     <row r="39" spans="1:21">
@@ -3434,8 +3470,8 @@
         <f>=IF(M39="是",D39-N39,0)</f>
         <v>0</v>
       </c>
-      <c r="S39" s="86" t="s"/>
-      <c r="T39" s="86" t="s"/>
+      <c r="S39" s="89" t="s"/>
+      <c r="T39" s="89" t="s"/>
       <c r="U39" s="35" t="s"/>
     </row>
     <row r="40" spans="1:21">
@@ -3474,8 +3510,8 @@
         <f>=IF(M40="是",D40-N40,0)</f>
         <v>0</v>
       </c>
-      <c r="S40" s="86" t="s"/>
-      <c r="T40" s="86" t="s"/>
+      <c r="S40" s="89" t="s"/>
+      <c r="T40" s="89" t="s"/>
       <c r="U40" s="35" t="s"/>
     </row>
     <row r="41" spans="1:21">
@@ -3514,8 +3550,8 @@
         <f>=IF(M41="是",D41-N41,0)</f>
         <v>0</v>
       </c>
-      <c r="S41" s="86" t="s"/>
-      <c r="T41" s="86" t="s"/>
+      <c r="S41" s="89" t="s"/>
+      <c r="T41" s="89" t="s"/>
       <c r="U41" s="35" t="s"/>
     </row>
     <row r="42" spans="1:21">
@@ -3554,8 +3590,8 @@
         <f>=IF(M42="是",D42-N42,0)</f>
         <v>0</v>
       </c>
-      <c r="S42" s="86" t="s"/>
-      <c r="T42" s="86" t="s"/>
+      <c r="S42" s="89" t="s"/>
+      <c r="T42" s="89" t="s"/>
       <c r="U42" s="35" t="s"/>
     </row>
     <row r="43" spans="1:21">
@@ -3594,8 +3630,8 @@
         <f>=IF(M43="是",D43-N43,0)</f>
         <v>0</v>
       </c>
-      <c r="S43" s="86" t="s"/>
-      <c r="T43" s="86" t="s"/>
+      <c r="S43" s="89" t="s"/>
+      <c r="T43" s="89" t="s"/>
       <c r="U43" s="35" t="s"/>
     </row>
     <row r="44" spans="1:21">
@@ -3634,8 +3670,8 @@
         <f>=IF(M44="是",D44-N44,0)</f>
         <v>0</v>
       </c>
-      <c r="S44" s="86" t="s"/>
-      <c r="T44" s="86" t="s"/>
+      <c r="S44" s="89" t="s"/>
+      <c r="T44" s="89" t="s"/>
       <c r="U44" s="35" t="s"/>
     </row>
     <row r="45" spans="1:21">
@@ -3674,8 +3710,8 @@
         <f>=IF(M45="是",D45-N45,0)</f>
         <v>0</v>
       </c>
-      <c r="S45" s="86" t="s"/>
-      <c r="T45" s="86" t="s"/>
+      <c r="S45" s="89" t="s"/>
+      <c r="T45" s="89" t="s"/>
       <c r="U45" s="35" t="s"/>
     </row>
     <row r="46" spans="1:21">
@@ -3714,8 +3750,8 @@
         <f>=IF(M46="是",D46-N46,0)</f>
         <v>0</v>
       </c>
-      <c r="S46" s="86" t="s"/>
-      <c r="T46" s="86" t="s"/>
+      <c r="S46" s="89" t="s"/>
+      <c r="T46" s="89" t="s"/>
       <c r="U46" s="35" t="s"/>
     </row>
     <row r="47" spans="1:21">
@@ -3754,8 +3790,8 @@
         <f>=IF(M47="是",D47-N47,0)</f>
         <v>0</v>
       </c>
-      <c r="S47" s="86" t="s"/>
-      <c r="T47" s="86" t="s"/>
+      <c r="S47" s="89" t="s"/>
+      <c r="T47" s="89" t="s"/>
       <c r="U47" s="35" t="s"/>
     </row>
     <row r="48" spans="1:21">
@@ -3794,8 +3830,8 @@
         <f>=IF(M48="是",D48-N48,0)</f>
         <v>0</v>
       </c>
-      <c r="S48" s="86" t="s"/>
-      <c r="T48" s="86" t="s"/>
+      <c r="S48" s="89" t="s"/>
+      <c r="T48" s="89" t="s"/>
       <c r="U48" s="35" t="s"/>
     </row>
     <row r="49" spans="1:21">
@@ -3834,8 +3870,8 @@
         <f>=IF(M49="是",D49-N49,0)</f>
         <v>0</v>
       </c>
-      <c r="S49" s="86" t="s"/>
-      <c r="T49" s="86" t="s"/>
+      <c r="S49" s="89" t="s"/>
+      <c r="T49" s="89" t="s"/>
       <c r="U49" s="35" t="s"/>
     </row>
     <row r="50" spans="1:21">
@@ -3874,7 +3910,7 @@
         <f>=IF(M50="是",D50-N50,0)</f>
         <v>0</v>
       </c>
-      <c r="S50" s="92" t="s"/>
+      <c r="S50" s="95" t="s"/>
       <c r="U50" s="35" t="s"/>
     </row>
     <row r="51" spans="1:21">
@@ -3913,7 +3949,7 @@
         <f>=IF(M51="是",D51-N51,0)</f>
         <v>0</v>
       </c>
-      <c r="S51" s="92" t="s"/>
+      <c r="S51" s="95" t="s"/>
       <c r="U51" s="35" t="s"/>
     </row>
     <row r="52" spans="1:21">
@@ -3952,7 +3988,7 @@
         <f>=IF(M52="是",D52-N52,0)</f>
         <v>0</v>
       </c>
-      <c r="S52" s="92" t="s"/>
+      <c r="S52" s="95" t="s"/>
       <c r="U52" s="35" t="s"/>
     </row>
     <row r="53" spans="1:21">
@@ -3991,7 +4027,7 @@
         <f>=IF(M53="是",D53-N53,0)</f>
         <v>0</v>
       </c>
-      <c r="S53" s="92" t="s"/>
+      <c r="S53" s="95" t="s"/>
       <c r="U53" s="35" t="s"/>
     </row>
     <row r="54" spans="1:21">
@@ -4030,7 +4066,7 @@
         <f>=IF(M54="是",D54-N54,0)</f>
         <v>0</v>
       </c>
-      <c r="S54" s="92" t="s"/>
+      <c r="S54" s="95" t="s"/>
       <c r="U54" s="35" t="s"/>
     </row>
     <row r="55" spans="1:21">
@@ -4069,7 +4105,7 @@
         <f>=IF(M55="是",D55-N55,0)</f>
         <v>0</v>
       </c>
-      <c r="S55" s="92" t="s"/>
+      <c r="S55" s="95" t="s"/>
       <c r="U55" s="35" t="s"/>
     </row>
     <row r="56" spans="1:21">
@@ -4108,7 +4144,7 @@
         <f>=IF(M56="是",D56-N56,0)</f>
         <v>0</v>
       </c>
-      <c r="S56" s="92" t="s"/>
+      <c r="S56" s="95" t="s"/>
       <c r="U56" s="35" t="s"/>
     </row>
     <row r="57" spans="1:21">
@@ -4147,7 +4183,7 @@
         <f>=IF(M57="是",D57-N57,0)</f>
         <v>0</v>
       </c>
-      <c r="S57" s="92" t="s"/>
+      <c r="S57" s="95" t="s"/>
       <c r="U57" s="35" t="s"/>
     </row>
     <row r="58" spans="1:21">
@@ -4186,7 +4222,7 @@
         <f>=IF(M58="是",D58-N58,0)</f>
         <v>0</v>
       </c>
-      <c r="S58" s="92" t="s"/>
+      <c r="S58" s="95" t="s"/>
       <c r="U58" s="35" t="s"/>
     </row>
     <row r="59" spans="1:21">
@@ -4225,7 +4261,7 @@
         <f>=IF(M59="是",D59-N59,0)</f>
         <v>0</v>
       </c>
-      <c r="S59" s="92" t="s"/>
+      <c r="S59" s="95" t="s"/>
       <c r="U59" s="35" t="s"/>
     </row>
     <row r="60" spans="1:21">
@@ -4264,7 +4300,7 @@
         <f>=IF(M60="是",D60-N60,0)</f>
         <v>0</v>
       </c>
-      <c r="S60" s="92" t="s"/>
+      <c r="S60" s="95" t="s"/>
       <c r="U60" s="35" t="s"/>
     </row>
     <row r="61" spans="1:21">
@@ -4303,7 +4339,7 @@
         <f>=IF(M61="是",D61-N61,0)</f>
         <v>0</v>
       </c>
-      <c r="S61" s="92" t="s"/>
+      <c r="S61" s="95" t="s"/>
       <c r="U61" s="35" t="s"/>
     </row>
     <row r="62" spans="1:21">
@@ -4342,7 +4378,7 @@
         <f>=IF(M62="是",D62-N62,0)</f>
         <v>0</v>
       </c>
-      <c r="S62" s="92" t="s"/>
+      <c r="S62" s="95" t="s"/>
       <c r="U62" s="35" t="s"/>
     </row>
     <row r="63" spans="1:21">
@@ -4381,7 +4417,7 @@
         <f>=IF(M63="是",D63-N63,0)</f>
         <v>0</v>
       </c>
-      <c r="S63" s="92" t="s"/>
+      <c r="S63" s="95" t="s"/>
       <c r="U63" s="35" t="s"/>
     </row>
     <row r="64" spans="1:21">
@@ -4397,7 +4433,7 @@
         <f>=D64-O64</f>
         <v>0</v>
       </c>
-      <c r="F64" s="93" t="s"/>
+      <c r="F64" s="96" t="s"/>
       <c r="G64" s="24" t="s"/>
       <c r="H64" s="29" t="s">
         <v>21</v>
@@ -4409,7 +4445,7 @@
         <v>45</v>
       </c>
       <c r="K64" s="25" t="s"/>
-      <c r="L64" s="94" t="s"/>
+      <c r="L64" s="97" t="s"/>
       <c r="M64" s="31" t="s">
         <v>50</v>
       </c>
@@ -4420,7 +4456,7 @@
         <f>=IF(M64="是",D64-N64,0)</f>
         <v>0</v>
       </c>
-      <c r="S64" s="92" t="s"/>
+      <c r="S64" s="95" t="s"/>
       <c r="U64" s="35" t="s"/>
     </row>
     <row r="65" spans="1:21">
@@ -4448,7 +4484,7 @@
         <v>45</v>
       </c>
       <c r="K65" s="11" t="s"/>
-      <c r="L65" s="95" t="s"/>
+      <c r="L65" s="98" t="s"/>
       <c r="M65" s="31" t="s">
         <v>50</v>
       </c>
@@ -4459,7 +4495,7 @@
         <f>=IF(M65="是",D65-N65,0)</f>
         <v>0</v>
       </c>
-      <c r="S65" s="92" t="s"/>
+      <c r="S65" s="95" t="s"/>
       <c r="U65" s="35" t="s"/>
     </row>
     <row r="66" spans="1:21">
@@ -4487,7 +4523,7 @@
         <v>45</v>
       </c>
       <c r="K66" s="11" t="s"/>
-      <c r="L66" s="95" t="s"/>
+      <c r="L66" s="98" t="s"/>
       <c r="M66" s="31" t="s">
         <v>50</v>
       </c>
@@ -4498,7 +4534,7 @@
         <f>=IF(M66="是",D66-N66,0)</f>
         <v>0</v>
       </c>
-      <c r="S66" s="92" t="s"/>
+      <c r="S66" s="95" t="s"/>
       <c r="U66" s="35" t="s"/>
     </row>
     <row r="67" spans="1:21">
@@ -4526,7 +4562,7 @@
         <v>45</v>
       </c>
       <c r="K67" s="11" t="s"/>
-      <c r="L67" s="95" t="s"/>
+      <c r="L67" s="98" t="s"/>
       <c r="M67" s="31" t="s">
         <v>50</v>
       </c>
@@ -4537,7 +4573,7 @@
         <f>=IF(M67="是",D67-N67,0)</f>
         <v>0</v>
       </c>
-      <c r="S67" s="92" t="s"/>
+      <c r="S67" s="95" t="s"/>
       <c r="U67" s="35" t="s"/>
     </row>
     <row r="68" spans="1:21">
@@ -4565,7 +4601,7 @@
         <v>45</v>
       </c>
       <c r="K68" s="11" t="s"/>
-      <c r="L68" s="95" t="s"/>
+      <c r="L68" s="98" t="s"/>
       <c r="M68" s="31" t="s">
         <v>50</v>
       </c>
@@ -4576,7 +4612,7 @@
         <f>=IF(M68="是",D68-N68,0)</f>
         <v>0</v>
       </c>
-      <c r="S68" s="92" t="s"/>
+      <c r="S68" s="95" t="s"/>
       <c r="U68" s="35" t="s"/>
     </row>
     <row r="69" spans="1:21">
@@ -4604,7 +4640,7 @@
         <v>45</v>
       </c>
       <c r="K69" s="11" t="s"/>
-      <c r="L69" s="95" t="s"/>
+      <c r="L69" s="98" t="s"/>
       <c r="M69" s="31" t="s">
         <v>50</v>
       </c>
@@ -4615,7 +4651,7 @@
         <f>=IF(M69="是",D69-N69,0)</f>
         <v>0</v>
       </c>
-      <c r="S69" s="92" t="s"/>
+      <c r="S69" s="95" t="s"/>
       <c r="U69" s="35" t="s"/>
     </row>
     <row r="70" spans="1:21">
@@ -4643,7 +4679,7 @@
         <v>45</v>
       </c>
       <c r="K70" s="11" t="s"/>
-      <c r="L70" s="95" t="s"/>
+      <c r="L70" s="98" t="s"/>
       <c r="M70" s="31" t="s">
         <v>50</v>
       </c>
@@ -4654,7 +4690,7 @@
         <f>=IF(M70="是",D70-N70,0)</f>
         <v>0</v>
       </c>
-      <c r="S70" s="92" t="s"/>
+      <c r="S70" s="95" t="s"/>
       <c r="U70" s="35" t="s"/>
     </row>
     <row r="71" spans="1:21">
@@ -4682,7 +4718,7 @@
         <v>45</v>
       </c>
       <c r="K71" s="11" t="s"/>
-      <c r="L71" s="95" t="s"/>
+      <c r="L71" s="98" t="s"/>
       <c r="M71" s="31" t="s">
         <v>50</v>
       </c>
@@ -4693,7 +4729,7 @@
         <f>=IF(M71="是",D71-N71,0)</f>
         <v>0</v>
       </c>
-      <c r="S71" s="92" t="s"/>
+      <c r="S71" s="95" t="s"/>
       <c r="U71" s="35" t="s"/>
     </row>
     <row r="72" spans="1:21">
@@ -4721,7 +4757,7 @@
         <v>45</v>
       </c>
       <c r="K72" s="11" t="s"/>
-      <c r="L72" s="95" t="s"/>
+      <c r="L72" s="98" t="s"/>
       <c r="M72" s="31" t="s">
         <v>50</v>
       </c>
@@ -4732,7 +4768,7 @@
         <f>=IF(M72="是",D72-N72,0)</f>
         <v>0</v>
       </c>
-      <c r="S72" s="92" t="s"/>
+      <c r="S72" s="95" t="s"/>
       <c r="U72" s="35" t="s"/>
     </row>
     <row r="73" spans="1:21">
@@ -4760,7 +4796,7 @@
         <v>45</v>
       </c>
       <c r="K73" s="11" t="s"/>
-      <c r="L73" s="95" t="s"/>
+      <c r="L73" s="98" t="s"/>
       <c r="M73" s="31" t="s">
         <v>50</v>
       </c>
@@ -4771,7 +4807,7 @@
         <f>=IF(M73="是",D73-N73,0)</f>
         <v>0</v>
       </c>
-      <c r="S73" s="92" t="s"/>
+      <c r="S73" s="95" t="s"/>
       <c r="U73" s="35" t="s"/>
     </row>
     <row r="74" spans="1:21">
@@ -4799,7 +4835,7 @@
         <v>45</v>
       </c>
       <c r="K74" s="11" t="s"/>
-      <c r="L74" s="95" t="s"/>
+      <c r="L74" s="98" t="s"/>
       <c r="M74" s="31" t="s">
         <v>50</v>
       </c>
@@ -4810,7 +4846,7 @@
         <f>=IF(M74="是",D74-N74,0)</f>
         <v>0</v>
       </c>
-      <c r="S74" s="92" t="s"/>
+      <c r="S74" s="95" t="s"/>
       <c r="U74" s="35" t="s"/>
     </row>
     <row r="75" spans="1:21">
@@ -4838,7 +4874,7 @@
         <v>45</v>
       </c>
       <c r="K75" s="11" t="s"/>
-      <c r="L75" s="95" t="s"/>
+      <c r="L75" s="98" t="s"/>
       <c r="M75" s="31" t="s">
         <v>50</v>
       </c>
@@ -4849,7 +4885,7 @@
         <f>=IF(M75="是",D75-N75,0)</f>
         <v>0</v>
       </c>
-      <c r="S75" s="92" t="s"/>
+      <c r="S75" s="95" t="s"/>
       <c r="U75" s="35" t="s"/>
     </row>
     <row r="76" spans="1:21">
@@ -4877,7 +4913,7 @@
         <v>45</v>
       </c>
       <c r="K76" s="11" t="s"/>
-      <c r="L76" s="95" t="s"/>
+      <c r="L76" s="98" t="s"/>
       <c r="M76" s="31" t="s">
         <v>50</v>
       </c>
@@ -4888,7 +4924,7 @@
         <f>=IF(M76="是",D76-N76,0)</f>
         <v>0</v>
       </c>
-      <c r="S76" s="92" t="s"/>
+      <c r="S76" s="95" t="s"/>
       <c r="U76" s="35" t="s"/>
     </row>
     <row r="77" spans="1:21">
@@ -4916,7 +4952,7 @@
         <v>45</v>
       </c>
       <c r="K77" s="11" t="s"/>
-      <c r="L77" s="95" t="s"/>
+      <c r="L77" s="98" t="s"/>
       <c r="M77" s="31" t="s">
         <v>50</v>
       </c>
@@ -4927,7 +4963,7 @@
         <f>=IF(M77="是",D77-N77,0)</f>
         <v>0</v>
       </c>
-      <c r="S77" s="92" t="s"/>
+      <c r="S77" s="95" t="s"/>
       <c r="U77" s="35" t="s"/>
     </row>
     <row r="78" spans="1:21">
@@ -4955,7 +4991,7 @@
         <v>45</v>
       </c>
       <c r="K78" s="11" t="s"/>
-      <c r="L78" s="95" t="s"/>
+      <c r="L78" s="98" t="s"/>
       <c r="M78" s="31" t="s">
         <v>50</v>
       </c>
@@ -4966,7 +5002,7 @@
         <f>=IF(M78="是",D78-N78,0)</f>
         <v>0</v>
       </c>
-      <c r="S78" s="92" t="s"/>
+      <c r="S78" s="95" t="s"/>
       <c r="U78" s="35" t="s"/>
     </row>
     <row r="79" spans="1:21">
@@ -4994,7 +5030,7 @@
         <v>45</v>
       </c>
       <c r="K79" s="11" t="s"/>
-      <c r="L79" s="95" t="s"/>
+      <c r="L79" s="98" t="s"/>
       <c r="M79" s="31" t="s">
         <v>50</v>
       </c>
@@ -5005,7 +5041,7 @@
         <f>=IF(M79="是",D79-N79,0)</f>
         <v>0</v>
       </c>
-      <c r="S79" s="92" t="s"/>
+      <c r="S79" s="95" t="s"/>
       <c r="U79" s="35" t="s"/>
     </row>
     <row r="80" spans="1:21">
@@ -5033,7 +5069,7 @@
         <v>45</v>
       </c>
       <c r="K80" s="11" t="s"/>
-      <c r="L80" s="95" t="s"/>
+      <c r="L80" s="98" t="s"/>
       <c r="M80" s="31" t="s">
         <v>50</v>
       </c>
@@ -5044,7 +5080,7 @@
         <f>=IF(M80="是",D80-N80,0)</f>
         <v>0</v>
       </c>
-      <c r="S80" s="92" t="s"/>
+      <c r="S80" s="95" t="s"/>
       <c r="U80" s="35" t="s"/>
     </row>
     <row r="81" spans="1:21">
@@ -5072,7 +5108,7 @@
         <v>45</v>
       </c>
       <c r="K81" s="11" t="s"/>
-      <c r="L81" s="95" t="s"/>
+      <c r="L81" s="98" t="s"/>
       <c r="M81" s="31" t="s">
         <v>50</v>
       </c>
@@ -5083,7 +5119,7 @@
         <f>=IF(M81="是",D81-N81,0)</f>
         <v>0</v>
       </c>
-      <c r="S81" s="92" t="s"/>
+      <c r="S81" s="95" t="s"/>
       <c r="U81" s="35" t="s"/>
     </row>
     <row r="82" spans="1:21">
@@ -5111,7 +5147,7 @@
         <v>45</v>
       </c>
       <c r="K82" s="11" t="s"/>
-      <c r="L82" s="95" t="s"/>
+      <c r="L82" s="98" t="s"/>
       <c r="M82" s="31" t="s">
         <v>50</v>
       </c>
@@ -5122,7 +5158,7 @@
         <f>=IF(M82="是",D82-N82,0)</f>
         <v>0</v>
       </c>
-      <c r="S82" s="92" t="s"/>
+      <c r="S82" s="95" t="s"/>
       <c r="U82" s="35" t="s"/>
     </row>
     <row r="83" spans="1:21">
@@ -5150,7 +5186,7 @@
         <v>45</v>
       </c>
       <c r="K83" s="11" t="s"/>
-      <c r="L83" s="95" t="s"/>
+      <c r="L83" s="98" t="s"/>
       <c r="M83" s="31" t="s">
         <v>50</v>
       </c>
@@ -5161,7 +5197,7 @@
         <f>=IF(M83="是",D83-N83,0)</f>
         <v>0</v>
       </c>
-      <c r="S83" s="92" t="s"/>
+      <c r="S83" s="95" t="s"/>
       <c r="U83" s="35" t="s"/>
     </row>
     <row r="84" spans="1:21">
@@ -5189,7 +5225,7 @@
         <v>45</v>
       </c>
       <c r="K84" s="11" t="s"/>
-      <c r="L84" s="95" t="s"/>
+      <c r="L84" s="98" t="s"/>
       <c r="M84" s="31" t="s">
         <v>50</v>
       </c>
@@ -5200,7 +5236,7 @@
         <f>=IF(M84="是",D84-N84,0)</f>
         <v>0</v>
       </c>
-      <c r="S84" s="92" t="s"/>
+      <c r="S84" s="95" t="s"/>
       <c r="U84" s="35" t="s"/>
     </row>
     <row r="85" spans="1:21">
@@ -5228,7 +5264,7 @@
         <v>45</v>
       </c>
       <c r="K85" s="11" t="s"/>
-      <c r="L85" s="95" t="s"/>
+      <c r="L85" s="98" t="s"/>
       <c r="M85" s="31" t="s">
         <v>50</v>
       </c>
@@ -5239,7 +5275,7 @@
         <f>=IF(M85="是",D85-N85,0)</f>
         <v>0</v>
       </c>
-      <c r="S85" s="92" t="s"/>
+      <c r="S85" s="95" t="s"/>
       <c r="U85" s="35" t="s"/>
     </row>
     <row r="86" spans="1:21">
@@ -5267,7 +5303,7 @@
         <v>45</v>
       </c>
       <c r="K86" s="11" t="s"/>
-      <c r="L86" s="95" t="s"/>
+      <c r="L86" s="98" t="s"/>
       <c r="M86" s="31" t="s">
         <v>50</v>
       </c>
@@ -5278,7 +5314,7 @@
         <f>=IF(M86="是",D86-N86,0)</f>
         <v>0</v>
       </c>
-      <c r="S86" s="92" t="s"/>
+      <c r="S86" s="95" t="s"/>
       <c r="U86" s="35" t="s"/>
     </row>
     <row r="87" spans="1:21">
@@ -5306,7 +5342,7 @@
         <v>45</v>
       </c>
       <c r="K87" s="11" t="s"/>
-      <c r="L87" s="95" t="s"/>
+      <c r="L87" s="98" t="s"/>
       <c r="M87" s="31" t="s">
         <v>50</v>
       </c>
@@ -5317,7 +5353,7 @@
         <f>=IF(M87="是",D87-N87,0)</f>
         <v>0</v>
       </c>
-      <c r="S87" s="92" t="s"/>
+      <c r="S87" s="95" t="s"/>
       <c r="U87" s="35" t="s"/>
     </row>
     <row r="88" spans="1:21">
@@ -5345,7 +5381,7 @@
         <v>45</v>
       </c>
       <c r="K88" s="11" t="s"/>
-      <c r="L88" s="95" t="s"/>
+      <c r="L88" s="98" t="s"/>
       <c r="M88" s="31" t="s">
         <v>50</v>
       </c>
@@ -5356,7 +5392,7 @@
         <f>=IF(M88="是",D88-N88,0)</f>
         <v>0</v>
       </c>
-      <c r="S88" s="92" t="s"/>
+      <c r="S88" s="95" t="s"/>
       <c r="U88" s="35" t="s"/>
     </row>
     <row r="89" spans="1:21">
@@ -5384,7 +5420,7 @@
         <v>45</v>
       </c>
       <c r="K89" s="11" t="s"/>
-      <c r="L89" s="95" t="s"/>
+      <c r="L89" s="98" t="s"/>
       <c r="M89" s="31" t="s">
         <v>50</v>
       </c>
@@ -5395,7 +5431,7 @@
         <f>=IF(M89="是",D89-N89,0)</f>
         <v>0</v>
       </c>
-      <c r="S89" s="92" t="s"/>
+      <c r="S89" s="95" t="s"/>
       <c r="U89" s="35" t="s"/>
     </row>
     <row r="90" spans="1:21">
@@ -5423,7 +5459,7 @@
         <v>45</v>
       </c>
       <c r="K90" s="11" t="s"/>
-      <c r="L90" s="95" t="s"/>
+      <c r="L90" s="98" t="s"/>
       <c r="M90" s="31" t="s">
         <v>50</v>
       </c>
@@ -5434,7 +5470,7 @@
         <f>=IF(M90="是",D90-N90,0)</f>
         <v>0</v>
       </c>
-      <c r="S90" s="92" t="s"/>
+      <c r="S90" s="95" t="s"/>
       <c r="U90" s="35" t="s"/>
     </row>
     <row r="91" spans="1:21">
@@ -5462,7 +5498,7 @@
         <v>45</v>
       </c>
       <c r="K91" s="11" t="s"/>
-      <c r="L91" s="95" t="s"/>
+      <c r="L91" s="98" t="s"/>
       <c r="M91" s="31" t="s">
         <v>50</v>
       </c>
@@ -5473,7 +5509,7 @@
         <f>=IF(M91="是",D91-N91,0)</f>
         <v>0</v>
       </c>
-      <c r="S91" s="92" t="s"/>
+      <c r="S91" s="95" t="s"/>
       <c r="U91" s="35" t="s"/>
     </row>
     <row r="92" spans="1:21">
@@ -5501,7 +5537,7 @@
         <v>45</v>
       </c>
       <c r="K92" s="11" t="s"/>
-      <c r="L92" s="95" t="s"/>
+      <c r="L92" s="98" t="s"/>
       <c r="M92" s="31" t="s">
         <v>50</v>
       </c>
@@ -5512,7 +5548,7 @@
         <f>=IF(M92="是",D92-N92,0)</f>
         <v>0</v>
       </c>
-      <c r="S92" s="92" t="s"/>
+      <c r="S92" s="95" t="s"/>
       <c r="U92" s="35" t="s"/>
     </row>
     <row r="93" spans="1:21">
@@ -5540,7 +5576,7 @@
         <v>45</v>
       </c>
       <c r="K93" s="11" t="s"/>
-      <c r="L93" s="95" t="s"/>
+      <c r="L93" s="98" t="s"/>
       <c r="M93" s="31" t="s">
         <v>50</v>
       </c>
@@ -5551,7 +5587,7 @@
         <f>=IF(M93="是",D93-N93,0)</f>
         <v>0</v>
       </c>
-      <c r="S93" s="92" t="s"/>
+      <c r="S93" s="95" t="s"/>
       <c r="U93" s="35" t="s"/>
     </row>
     <row r="94" spans="1:21">
@@ -5579,7 +5615,7 @@
         <v>45</v>
       </c>
       <c r="K94" s="11" t="s"/>
-      <c r="L94" s="95" t="s"/>
+      <c r="L94" s="98" t="s"/>
       <c r="M94" s="31" t="s">
         <v>50</v>
       </c>
@@ -5590,7 +5626,7 @@
         <f>=IF(M94="是",D94-N94,0)</f>
         <v>0</v>
       </c>
-      <c r="S94" s="92" t="s"/>
+      <c r="S94" s="95" t="s"/>
       <c r="U94" s="35" t="s"/>
     </row>
     <row r="95" spans="1:21">
@@ -5618,7 +5654,7 @@
         <v>45</v>
       </c>
       <c r="K95" s="11" t="s"/>
-      <c r="L95" s="95" t="s"/>
+      <c r="L95" s="98" t="s"/>
       <c r="M95" s="31" t="s">
         <v>50</v>
       </c>
@@ -5629,7 +5665,7 @@
         <f>=IF(M95="是",D95-N95,0)</f>
         <v>0</v>
       </c>
-      <c r="S95" s="92" t="s"/>
+      <c r="S95" s="95" t="s"/>
       <c r="U95" s="35" t="s"/>
     </row>
     <row r="96" spans="1:21">
@@ -5657,7 +5693,7 @@
         <v>45</v>
       </c>
       <c r="K96" s="11" t="s"/>
-      <c r="L96" s="95" t="s"/>
+      <c r="L96" s="98" t="s"/>
       <c r="M96" s="31" t="s">
         <v>50</v>
       </c>
@@ -5668,7 +5704,7 @@
         <f>=IF(M96="是",D96-N96,0)</f>
         <v>0</v>
       </c>
-      <c r="S96" s="92" t="s"/>
+      <c r="S96" s="95" t="s"/>
       <c r="U96" s="35" t="s"/>
     </row>
     <row r="97" spans="1:21">
@@ -5696,7 +5732,7 @@
         <v>45</v>
       </c>
       <c r="K97" s="11" t="s"/>
-      <c r="L97" s="95" t="s"/>
+      <c r="L97" s="98" t="s"/>
       <c r="M97" s="31" t="s">
         <v>50</v>
       </c>
@@ -5707,7 +5743,7 @@
         <f>=IF(M97="是",D97-N97,0)</f>
         <v>0</v>
       </c>
-      <c r="S97" s="92" t="s"/>
+      <c r="S97" s="95" t="s"/>
       <c r="U97" s="35" t="s"/>
     </row>
     <row r="98" spans="1:21">
@@ -5735,7 +5771,7 @@
         <v>45</v>
       </c>
       <c r="K98" s="11" t="s"/>
-      <c r="L98" s="95" t="s"/>
+      <c r="L98" s="98" t="s"/>
       <c r="M98" s="31" t="s">
         <v>50</v>
       </c>
@@ -5746,7 +5782,7 @@
         <f>=IF(M98="是",D98-N98,0)</f>
         <v>0</v>
       </c>
-      <c r="S98" s="92" t="s"/>
+      <c r="S98" s="95" t="s"/>
       <c r="U98" s="35" t="s"/>
     </row>
     <row r="99" spans="1:21">
@@ -5774,7 +5810,7 @@
         <v>45</v>
       </c>
       <c r="K99" s="11" t="s"/>
-      <c r="L99" s="95" t="s"/>
+      <c r="L99" s="98" t="s"/>
       <c r="M99" s="31" t="s">
         <v>50</v>
       </c>
@@ -5785,7 +5821,7 @@
         <f>=IF(M99="是",D99-N99,0)</f>
         <v>0</v>
       </c>
-      <c r="S99" s="92" t="s"/>
+      <c r="S99" s="95" t="s"/>
       <c r="U99" s="35" t="s"/>
     </row>
     <row r="100" spans="1:21">
@@ -5813,7 +5849,7 @@
         <v>45</v>
       </c>
       <c r="K100" s="11" t="s"/>
-      <c r="L100" s="95" t="s"/>
+      <c r="L100" s="98" t="s"/>
       <c r="M100" s="31" t="s">
         <v>50</v>
       </c>
@@ -5824,7 +5860,7 @@
         <f>=IF(M100="是",D100-N100,0)</f>
         <v>0</v>
       </c>
-      <c r="S100" s="92" t="s"/>
+      <c r="S100" s="95" t="s"/>
       <c r="U100" s="35" t="s"/>
     </row>
     <row r="101" spans="1:21">
@@ -5852,7 +5888,7 @@
         <v>45</v>
       </c>
       <c r="K101" s="11" t="s"/>
-      <c r="L101" s="95" t="s"/>
+      <c r="L101" s="98" t="s"/>
       <c r="M101" s="31" t="s">
         <v>50</v>
       </c>
@@ -5863,7 +5899,7 @@
         <f>=IF(M101="是",D101-N101,0)</f>
         <v>0</v>
       </c>
-      <c r="S101" s="92" t="s"/>
+      <c r="S101" s="95" t="s"/>
       <c r="U101" s="35" t="s"/>
     </row>
     <row r="102" spans="1:21">
@@ -5891,7 +5927,7 @@
         <v>45</v>
       </c>
       <c r="K102" s="11" t="s"/>
-      <c r="L102" s="95" t="s"/>
+      <c r="L102" s="98" t="s"/>
       <c r="M102" s="31" t="s">
         <v>50</v>
       </c>
@@ -5902,7 +5938,7 @@
         <f>=IF(M102="是",D102-N102,0)</f>
         <v>0</v>
       </c>
-      <c r="S102" s="92" t="s"/>
+      <c r="S102" s="95" t="s"/>
       <c r="U102" s="35" t="s"/>
     </row>
     <row r="103" spans="1:21">
@@ -5930,7 +5966,7 @@
         <v>45</v>
       </c>
       <c r="K103" s="11" t="s"/>
-      <c r="L103" s="95" t="s"/>
+      <c r="L103" s="98" t="s"/>
       <c r="M103" s="31" t="s">
         <v>50</v>
       </c>
@@ -5941,7 +5977,7 @@
         <f>=IF(M103="是",D103-N103,0)</f>
         <v>0</v>
       </c>
-      <c r="S103" s="92" t="s"/>
+      <c r="S103" s="95" t="s"/>
       <c r="U103" s="35" t="s"/>
     </row>
     <row r="104" spans="1:21">
@@ -5969,7 +6005,7 @@
         <v>45</v>
       </c>
       <c r="K104" s="11" t="s"/>
-      <c r="L104" s="95" t="s"/>
+      <c r="L104" s="98" t="s"/>
       <c r="M104" s="31" t="s">
         <v>50</v>
       </c>
@@ -5980,7 +6016,7 @@
         <f>=IF(M104="是",D104-N104,0)</f>
         <v>0</v>
       </c>
-      <c r="S104" s="92" t="s"/>
+      <c r="S104" s="95" t="s"/>
       <c r="U104" s="35" t="s"/>
     </row>
     <row r="105" spans="1:21">
@@ -6008,7 +6044,7 @@
         <v>45</v>
       </c>
       <c r="K105" s="11" t="s"/>
-      <c r="L105" s="95" t="s"/>
+      <c r="L105" s="98" t="s"/>
       <c r="M105" s="31" t="s">
         <v>50</v>
       </c>
@@ -6019,7 +6055,7 @@
         <f>=IF(M105="是",D105-N105,0)</f>
         <v>0</v>
       </c>
-      <c r="S105" s="92" t="s"/>
+      <c r="S105" s="95" t="s"/>
       <c r="U105" s="35" t="s"/>
     </row>
     <row r="106" spans="1:21">
@@ -6047,7 +6083,7 @@
         <v>45</v>
       </c>
       <c r="K106" s="11" t="s"/>
-      <c r="L106" s="95" t="s"/>
+      <c r="L106" s="98" t="s"/>
       <c r="M106" s="31" t="s">
         <v>50</v>
       </c>
@@ -6058,7 +6094,7 @@
         <f>=IF(M106="是",D106-N106,0)</f>
         <v>0</v>
       </c>
-      <c r="S106" s="92" t="s"/>
+      <c r="S106" s="95" t="s"/>
       <c r="U106" s="35" t="s"/>
     </row>
     <row r="107" spans="1:21">
@@ -6086,7 +6122,7 @@
         <v>45</v>
       </c>
       <c r="K107" s="11" t="s"/>
-      <c r="L107" s="95" t="s"/>
+      <c r="L107" s="98" t="s"/>
       <c r="M107" s="31" t="s">
         <v>50</v>
       </c>
@@ -6097,7 +6133,7 @@
         <f>=IF(M107="是",D107-N107,0)</f>
         <v>0</v>
       </c>
-      <c r="S107" s="92" t="s"/>
+      <c r="S107" s="95" t="s"/>
       <c r="U107" s="35" t="s"/>
     </row>
     <row r="108" spans="1:21">
@@ -6125,7 +6161,7 @@
         <v>45</v>
       </c>
       <c r="K108" s="11" t="s"/>
-      <c r="L108" s="95" t="s"/>
+      <c r="L108" s="98" t="s"/>
       <c r="M108" s="31" t="s">
         <v>50</v>
       </c>
@@ -6136,7 +6172,7 @@
         <f>=IF(M108="是",D108-N108,0)</f>
         <v>0</v>
       </c>
-      <c r="S108" s="92" t="s"/>
+      <c r="S108" s="95" t="s"/>
       <c r="U108" s="35" t="s"/>
     </row>
     <row r="109" spans="1:21">
@@ -6164,7 +6200,7 @@
         <v>45</v>
       </c>
       <c r="K109" s="11" t="s"/>
-      <c r="L109" s="95" t="s"/>
+      <c r="L109" s="98" t="s"/>
       <c r="M109" s="31" t="s">
         <v>50</v>
       </c>
@@ -6175,7 +6211,7 @@
         <f>=IF(M109="是",D109-N109,0)</f>
         <v>0</v>
       </c>
-      <c r="S109" s="92" t="s"/>
+      <c r="S109" s="95" t="s"/>
       <c r="U109" s="35" t="s"/>
     </row>
     <row r="110" spans="1:21">
@@ -6203,7 +6239,7 @@
         <v>45</v>
       </c>
       <c r="K110" s="11" t="s"/>
-      <c r="L110" s="95" t="s"/>
+      <c r="L110" s="98" t="s"/>
       <c r="M110" s="31" t="s">
         <v>50</v>
       </c>
@@ -6214,7 +6250,7 @@
         <f>=IF(M110="是",D110-N110,0)</f>
         <v>0</v>
       </c>
-      <c r="S110" s="92" t="s"/>
+      <c r="S110" s="95" t="s"/>
       <c r="U110" s="35" t="s"/>
     </row>
     <row r="111" spans="1:21">
@@ -6242,7 +6278,7 @@
         <v>45</v>
       </c>
       <c r="K111" s="11" t="s"/>
-      <c r="L111" s="95" t="s"/>
+      <c r="L111" s="98" t="s"/>
       <c r="M111" s="31" t="s">
         <v>50</v>
       </c>
@@ -6253,7 +6289,7 @@
         <f>=IF(M111="是",D111-N111,0)</f>
         <v>0</v>
       </c>
-      <c r="S111" s="92" t="s"/>
+      <c r="S111" s="95" t="s"/>
       <c r="U111" s="35" t="s"/>
     </row>
     <row r="112" spans="1:21">
@@ -6281,7 +6317,7 @@
         <v>45</v>
       </c>
       <c r="K112" s="11" t="s"/>
-      <c r="L112" s="95" t="s"/>
+      <c r="L112" s="98" t="s"/>
       <c r="M112" s="31" t="s">
         <v>50</v>
       </c>
@@ -6292,7 +6328,7 @@
         <f>=IF(M112="是",D112-N112,0)</f>
         <v>0</v>
       </c>
-      <c r="S112" s="92" t="s"/>
+      <c r="S112" s="95" t="s"/>
       <c r="U112" s="35" t="s"/>
     </row>
     <row r="113" spans="1:21">
@@ -6320,7 +6356,7 @@
         <v>45</v>
       </c>
       <c r="K113" s="11" t="s"/>
-      <c r="L113" s="95" t="s"/>
+      <c r="L113" s="98" t="s"/>
       <c r="M113" s="31" t="s">
         <v>50</v>
       </c>
@@ -6331,7 +6367,7 @@
         <f>=IF(M113="是",D113-N113,0)</f>
         <v>0</v>
       </c>
-      <c r="S113" s="92" t="s"/>
+      <c r="S113" s="95" t="s"/>
       <c r="U113" s="35" t="s"/>
     </row>
     <row r="114" spans="1:21">
@@ -6359,7 +6395,7 @@
         <v>45</v>
       </c>
       <c r="K114" s="11" t="s"/>
-      <c r="L114" s="95" t="s"/>
+      <c r="L114" s="98" t="s"/>
       <c r="M114" s="31" t="s">
         <v>50</v>
       </c>
@@ -6370,7 +6406,7 @@
         <f>=IF(M114="是",D114-N114,0)</f>
         <v>0</v>
       </c>
-      <c r="S114" s="92" t="s"/>
+      <c r="S114" s="95" t="s"/>
       <c r="U114" s="35" t="s"/>
     </row>
     <row r="115" spans="1:21">
@@ -6398,7 +6434,7 @@
         <v>45</v>
       </c>
       <c r="K115" s="11" t="s"/>
-      <c r="L115" s="95" t="s"/>
+      <c r="L115" s="98" t="s"/>
       <c r="M115" s="31" t="s">
         <v>50</v>
       </c>
@@ -6409,7 +6445,7 @@
         <f>=IF(M115="是",D115-N115,0)</f>
         <v>0</v>
       </c>
-      <c r="S115" s="92" t="s"/>
+      <c r="S115" s="95" t="s"/>
       <c r="U115" s="35" t="s"/>
     </row>
     <row r="116" spans="1:21">
@@ -6437,7 +6473,7 @@
         <v>45</v>
       </c>
       <c r="K116" s="11" t="s"/>
-      <c r="L116" s="95" t="s"/>
+      <c r="L116" s="98" t="s"/>
       <c r="M116" s="31" t="s">
         <v>50</v>
       </c>
@@ -6448,7 +6484,7 @@
         <f>=IF(M116="是",D116-N116,0)</f>
         <v>0</v>
       </c>
-      <c r="S116" s="92" t="s"/>
+      <c r="S116" s="95" t="s"/>
       <c r="U116" s="35" t="s"/>
     </row>
     <row r="117" spans="1:21">
@@ -6476,7 +6512,7 @@
         <v>45</v>
       </c>
       <c r="K117" s="11" t="s"/>
-      <c r="L117" s="95" t="s"/>
+      <c r="L117" s="98" t="s"/>
       <c r="M117" s="31" t="s">
         <v>50</v>
       </c>
@@ -6487,7 +6523,7 @@
         <f>=IF(M117="是",D117-N117,0)</f>
         <v>0</v>
       </c>
-      <c r="S117" s="92" t="s"/>
+      <c r="S117" s="95" t="s"/>
       <c r="U117" s="35" t="s"/>
     </row>
     <row r="118" spans="1:21">
@@ -6515,7 +6551,7 @@
         <v>45</v>
       </c>
       <c r="K118" s="11" t="s"/>
-      <c r="L118" s="95" t="s"/>
+      <c r="L118" s="98" t="s"/>
       <c r="M118" s="31" t="s">
         <v>50</v>
       </c>
@@ -6526,7 +6562,7 @@
         <f>=IF(M118="是",D118-N118,0)</f>
         <v>0</v>
       </c>
-      <c r="S118" s="92" t="s"/>
+      <c r="S118" s="95" t="s"/>
       <c r="U118" s="35" t="s"/>
     </row>
     <row r="119" spans="1:21">
@@ -6554,7 +6590,7 @@
         <v>45</v>
       </c>
       <c r="K119" s="11" t="s"/>
-      <c r="L119" s="95" t="s"/>
+      <c r="L119" s="98" t="s"/>
       <c r="M119" s="31" t="s">
         <v>50</v>
       </c>
@@ -6565,7 +6601,7 @@
         <f>=IF(M119="是",D119-N119,0)</f>
         <v>0</v>
       </c>
-      <c r="S119" s="92" t="s"/>
+      <c r="S119" s="95" t="s"/>
       <c r="U119" s="35" t="s"/>
     </row>
     <row r="120" spans="1:21">
@@ -6593,7 +6629,7 @@
         <v>45</v>
       </c>
       <c r="K120" s="11" t="s"/>
-      <c r="L120" s="95" t="s"/>
+      <c r="L120" s="98" t="s"/>
       <c r="M120" s="31" t="s">
         <v>50</v>
       </c>
@@ -6604,7 +6640,7 @@
         <f>=IF(M120="是",D120-N120,0)</f>
         <v>0</v>
       </c>
-      <c r="S120" s="92" t="s"/>
+      <c r="S120" s="95" t="s"/>
       <c r="U120" s="35" t="s"/>
     </row>
     <row r="121" spans="1:21">
@@ -6632,7 +6668,7 @@
         <v>45</v>
       </c>
       <c r="K121" s="11" t="s"/>
-      <c r="L121" s="95" t="s"/>
+      <c r="L121" s="98" t="s"/>
       <c r="M121" s="31" t="s">
         <v>50</v>
       </c>
@@ -6643,7 +6679,7 @@
         <f>=IF(M121="是",D121-N121,0)</f>
         <v>0</v>
       </c>
-      <c r="S121" s="92" t="s"/>
+      <c r="S121" s="95" t="s"/>
       <c r="U121" s="35" t="s"/>
     </row>
     <row r="122" spans="1:21">
@@ -6671,7 +6707,7 @@
         <v>45</v>
       </c>
       <c r="K122" s="11" t="s"/>
-      <c r="L122" s="95" t="s"/>
+      <c r="L122" s="98" t="s"/>
       <c r="M122" s="31" t="s">
         <v>50</v>
       </c>
@@ -6682,7 +6718,7 @@
         <f>=IF(M122="是",D122-N122,0)</f>
         <v>0</v>
       </c>
-      <c r="S122" s="92" t="s"/>
+      <c r="S122" s="95" t="s"/>
       <c r="U122" s="35" t="s"/>
     </row>
     <row r="123" spans="1:21">
@@ -6710,7 +6746,7 @@
         <v>45</v>
       </c>
       <c r="K123" s="11" t="s"/>
-      <c r="L123" s="95" t="s"/>
+      <c r="L123" s="98" t="s"/>
       <c r="M123" s="31" t="s">
         <v>50</v>
       </c>
@@ -6721,7 +6757,7 @@
         <f>=IF(M123="是",D123-N123,0)</f>
         <v>0</v>
       </c>
-      <c r="S123" s="92" t="s"/>
+      <c r="S123" s="95" t="s"/>
       <c r="U123" s="35" t="s"/>
     </row>
     <row r="124" spans="1:21">
@@ -6749,7 +6785,7 @@
         <v>45</v>
       </c>
       <c r="K124" s="11" t="s"/>
-      <c r="L124" s="95" t="s"/>
+      <c r="L124" s="98" t="s"/>
       <c r="M124" s="31" t="s">
         <v>50</v>
       </c>
@@ -6760,7 +6796,7 @@
         <f>=IF(M124="是",D124-N124,0)</f>
         <v>0</v>
       </c>
-      <c r="S124" s="92" t="s"/>
+      <c r="S124" s="95" t="s"/>
       <c r="U124" s="35" t="s"/>
     </row>
     <row r="125" spans="1:21">
@@ -6788,7 +6824,7 @@
         <v>45</v>
       </c>
       <c r="K125" s="11" t="s"/>
-      <c r="L125" s="95" t="s"/>
+      <c r="L125" s="98" t="s"/>
       <c r="M125" s="31" t="s">
         <v>50</v>
       </c>
@@ -6799,7 +6835,7 @@
         <f>=IF(M125="是",D125-N125,0)</f>
         <v>0</v>
       </c>
-      <c r="S125" s="92" t="s"/>
+      <c r="S125" s="95" t="s"/>
       <c r="U125" s="35" t="s"/>
     </row>
     <row r="126" spans="1:21">
@@ -6827,7 +6863,7 @@
         <v>45</v>
       </c>
       <c r="K126" s="11" t="s"/>
-      <c r="L126" s="95" t="s"/>
+      <c r="L126" s="98" t="s"/>
       <c r="M126" s="31" t="s">
         <v>50</v>
       </c>
@@ -6838,7 +6874,7 @@
         <f>=IF(M126="是",D126-N126,0)</f>
         <v>0</v>
       </c>
-      <c r="S126" s="92" t="s"/>
+      <c r="S126" s="95" t="s"/>
       <c r="U126" s="35" t="s"/>
     </row>
     <row r="127" spans="1:21">
@@ -6866,7 +6902,7 @@
         <v>45</v>
       </c>
       <c r="K127" s="11" t="s"/>
-      <c r="L127" s="95" t="s"/>
+      <c r="L127" s="98" t="s"/>
       <c r="M127" s="31" t="s">
         <v>50</v>
       </c>
@@ -6877,7 +6913,7 @@
         <f>=IF(M127="是",D127-N127,0)</f>
         <v>0</v>
       </c>
-      <c r="S127" s="92" t="s"/>
+      <c r="S127" s="95" t="s"/>
       <c r="U127" s="35" t="s"/>
     </row>
     <row r="128" spans="1:21">
@@ -6905,7 +6941,7 @@
         <v>45</v>
       </c>
       <c r="K128" s="11" t="s"/>
-      <c r="L128" s="95" t="s"/>
+      <c r="L128" s="98" t="s"/>
       <c r="M128" s="31" t="s">
         <v>50</v>
       </c>
@@ -6916,7 +6952,7 @@
         <f>=IF(M128="是",D128-N128,0)</f>
         <v>0</v>
       </c>
-      <c r="S128" s="92" t="s"/>
+      <c r="S128" s="95" t="s"/>
       <c r="U128" s="35" t="s"/>
     </row>
     <row r="129" spans="1:21">
@@ -6944,7 +6980,7 @@
         <v>45</v>
       </c>
       <c r="K129" s="11" t="s"/>
-      <c r="L129" s="95" t="s"/>
+      <c r="L129" s="98" t="s"/>
       <c r="M129" s="31" t="s">
         <v>50</v>
       </c>
@@ -6955,7 +6991,7 @@
         <f>=IF(M129="是",D129-N129,0)</f>
         <v>0</v>
       </c>
-      <c r="S129" s="92" t="s"/>
+      <c r="S129" s="95" t="s"/>
       <c r="U129" s="35" t="s"/>
     </row>
     <row r="130" spans="1:21">
@@ -6983,7 +7019,7 @@
         <v>45</v>
       </c>
       <c r="K130" s="11" t="s"/>
-      <c r="L130" s="95" t="s"/>
+      <c r="L130" s="98" t="s"/>
       <c r="M130" s="31" t="s">
         <v>50</v>
       </c>
@@ -6994,7 +7030,7 @@
         <f>=IF(M130="是",D130-N130,0)</f>
         <v>0</v>
       </c>
-      <c r="S130" s="92" t="s"/>
+      <c r="S130" s="95" t="s"/>
       <c r="U130" s="35" t="s"/>
     </row>
     <row r="131" spans="1:21">
@@ -7022,7 +7058,7 @@
         <v>45</v>
       </c>
       <c r="K131" s="11" t="s"/>
-      <c r="L131" s="95" t="s"/>
+      <c r="L131" s="98" t="s"/>
       <c r="M131" s="31" t="s">
         <v>50</v>
       </c>
@@ -7033,7 +7069,7 @@
         <f>=IF(M131="是",D131-N131,0)</f>
         <v>0</v>
       </c>
-      <c r="S131" s="92" t="s"/>
+      <c r="S131" s="95" t="s"/>
       <c r="U131" s="35" t="s"/>
     </row>
     <row r="132" spans="1:21">
@@ -7061,7 +7097,7 @@
         <v>45</v>
       </c>
       <c r="K132" s="11" t="s"/>
-      <c r="L132" s="95" t="s"/>
+      <c r="L132" s="98" t="s"/>
       <c r="M132" s="31" t="s">
         <v>50</v>
       </c>
@@ -7072,7 +7108,7 @@
         <f>=IF(M132="是",D132-N132,0)</f>
         <v>0</v>
       </c>
-      <c r="S132" s="92" t="s"/>
+      <c r="S132" s="95" t="s"/>
       <c r="U132" s="35" t="s"/>
     </row>
     <row r="133" spans="1:21">
@@ -7100,7 +7136,7 @@
         <v>45</v>
       </c>
       <c r="K133" s="11" t="s"/>
-      <c r="L133" s="95" t="s"/>
+      <c r="L133" s="98" t="s"/>
       <c r="M133" s="31" t="s">
         <v>50</v>
       </c>
@@ -7111,7 +7147,7 @@
         <f>=IF(M133="是",D133-N133,0)</f>
         <v>0</v>
       </c>
-      <c r="S133" s="92" t="s"/>
+      <c r="S133" s="95" t="s"/>
       <c r="U133" s="35" t="s"/>
     </row>
     <row r="134" spans="1:21">
@@ -7139,7 +7175,7 @@
         <v>45</v>
       </c>
       <c r="K134" s="11" t="s"/>
-      <c r="L134" s="95" t="s"/>
+      <c r="L134" s="98" t="s"/>
       <c r="M134" s="31" t="s">
         <v>50</v>
       </c>
@@ -7150,7 +7186,7 @@
         <f>=IF(M134="是",D134-N134,0)</f>
         <v>0</v>
       </c>
-      <c r="S134" s="92" t="s"/>
+      <c r="S134" s="95" t="s"/>
       <c r="U134" s="35" t="s"/>
     </row>
     <row r="135" spans="1:21">
@@ -7178,7 +7214,7 @@
         <v>45</v>
       </c>
       <c r="K135" s="11" t="s"/>
-      <c r="L135" s="95" t="s"/>
+      <c r="L135" s="98" t="s"/>
       <c r="M135" s="31" t="s">
         <v>50</v>
       </c>
@@ -7189,7 +7225,7 @@
         <f>=IF(M135="是",D135-N135,0)</f>
         <v>0</v>
       </c>
-      <c r="S135" s="92" t="s"/>
+      <c r="S135" s="95" t="s"/>
       <c r="U135" s="35" t="s"/>
     </row>
     <row r="136" spans="1:21">
@@ -7217,7 +7253,7 @@
         <v>45</v>
       </c>
       <c r="K136" s="11" t="s"/>
-      <c r="L136" s="95" t="s"/>
+      <c r="L136" s="98" t="s"/>
       <c r="M136" s="31" t="s">
         <v>50</v>
       </c>
@@ -7228,7 +7264,7 @@
         <f>=IF(M136="是",D136-N136,0)</f>
         <v>0</v>
       </c>
-      <c r="S136" s="92" t="s"/>
+      <c r="S136" s="95" t="s"/>
       <c r="U136" s="35" t="s"/>
     </row>
     <row r="137" spans="1:21">
@@ -7256,7 +7292,7 @@
         <v>45</v>
       </c>
       <c r="K137" s="11" t="s"/>
-      <c r="L137" s="95" t="s"/>
+      <c r="L137" s="98" t="s"/>
       <c r="M137" s="31" t="s">
         <v>50</v>
       </c>
@@ -7267,7 +7303,7 @@
         <f>=IF(M137="是",D137-N137,0)</f>
         <v>0</v>
       </c>
-      <c r="S137" s="92" t="s"/>
+      <c r="S137" s="95" t="s"/>
       <c r="U137" s="35" t="s"/>
     </row>
     <row r="138" spans="1:21">
@@ -7295,7 +7331,7 @@
         <v>45</v>
       </c>
       <c r="K138" s="11" t="s"/>
-      <c r="L138" s="95" t="s"/>
+      <c r="L138" s="98" t="s"/>
       <c r="M138" s="31" t="s">
         <v>50</v>
       </c>
@@ -7306,7 +7342,7 @@
         <f>=IF(M138="是",D138-N138,0)</f>
         <v>0</v>
       </c>
-      <c r="S138" s="92" t="s"/>
+      <c r="S138" s="95" t="s"/>
       <c r="U138" s="35" t="s"/>
     </row>
     <row r="139" spans="1:21">
@@ -7334,7 +7370,7 @@
         <v>45</v>
       </c>
       <c r="K139" s="11" t="s"/>
-      <c r="L139" s="95" t="s"/>
+      <c r="L139" s="98" t="s"/>
       <c r="M139" s="31" t="s">
         <v>50</v>
       </c>
@@ -7345,7 +7381,7 @@
         <f>=IF(M139="是",D139-N139,0)</f>
         <v>0</v>
       </c>
-      <c r="S139" s="92" t="s"/>
+      <c r="S139" s="95" t="s"/>
       <c r="U139" s="35" t="s"/>
     </row>
     <row r="140" spans="1:21">
@@ -7373,7 +7409,7 @@
         <v>45</v>
       </c>
       <c r="K140" s="11" t="s"/>
-      <c r="L140" s="95" t="s"/>
+      <c r="L140" s="98" t="s"/>
       <c r="M140" s="31" t="s">
         <v>50</v>
       </c>
@@ -7384,7 +7420,7 @@
         <f>=IF(M140="是",D140-N140,0)</f>
         <v>0</v>
       </c>
-      <c r="S140" s="92" t="s"/>
+      <c r="S140" s="95" t="s"/>
       <c r="U140" s="35" t="s"/>
     </row>
     <row r="141" spans="1:21">
@@ -7412,7 +7448,7 @@
         <v>45</v>
       </c>
       <c r="K141" s="11" t="s"/>
-      <c r="L141" s="95" t="s"/>
+      <c r="L141" s="98" t="s"/>
       <c r="M141" s="31" t="s">
         <v>50</v>
       </c>
@@ -7423,7 +7459,7 @@
         <f>=IF(M141="是",D141-N141,0)</f>
         <v>0</v>
       </c>
-      <c r="S141" s="92" t="s"/>
+      <c r="S141" s="95" t="s"/>
       <c r="U141" s="35" t="s"/>
     </row>
     <row r="142" spans="1:21">
@@ -7451,7 +7487,7 @@
         <v>45</v>
       </c>
       <c r="K142" s="11" t="s"/>
-      <c r="L142" s="95" t="s"/>
+      <c r="L142" s="98" t="s"/>
       <c r="M142" s="31" t="s">
         <v>50</v>
       </c>
@@ -7462,7 +7498,7 @@
         <f>=IF(M142="是",D142-N142,0)</f>
         <v>0</v>
       </c>
-      <c r="S142" s="92" t="s"/>
+      <c r="S142" s="95" t="s"/>
       <c r="U142" s="35" t="s"/>
     </row>
     <row r="143" spans="1:21">
@@ -7490,7 +7526,7 @@
         <v>45</v>
       </c>
       <c r="K143" s="11" t="s"/>
-      <c r="L143" s="95" t="s"/>
+      <c r="L143" s="98" t="s"/>
       <c r="M143" s="31" t="s">
         <v>50</v>
       </c>
@@ -7501,7 +7537,7 @@
         <f>=IF(M143="是",D143-N143,0)</f>
         <v>0</v>
       </c>
-      <c r="S143" s="92" t="s"/>
+      <c r="S143" s="95" t="s"/>
       <c r="U143" s="35" t="s"/>
     </row>
     <row r="144" spans="1:21">
@@ -7529,7 +7565,7 @@
         <v>45</v>
       </c>
       <c r="K144" s="11" t="s"/>
-      <c r="L144" s="95" t="s"/>
+      <c r="L144" s="98" t="s"/>
       <c r="M144" s="31" t="s">
         <v>50</v>
       </c>
@@ -7540,7 +7576,7 @@
         <f>=IF(M144="是",D144-N144,0)</f>
         <v>0</v>
       </c>
-      <c r="S144" s="92" t="s"/>
+      <c r="S144" s="95" t="s"/>
       <c r="U144" s="35" t="s"/>
     </row>
     <row r="145" spans="1:21">
@@ -7568,7 +7604,7 @@
         <v>45</v>
       </c>
       <c r="K145" s="11" t="s"/>
-      <c r="L145" s="95" t="s"/>
+      <c r="L145" s="98" t="s"/>
       <c r="M145" s="31" t="s">
         <v>50</v>
       </c>
@@ -7579,7 +7615,7 @@
         <f>=IF(M145="是",D145-N145,0)</f>
         <v>0</v>
       </c>
-      <c r="S145" s="92" t="s"/>
+      <c r="S145" s="95" t="s"/>
       <c r="U145" s="35" t="s"/>
     </row>
     <row r="146" spans="1:21">
@@ -7607,7 +7643,7 @@
         <v>45</v>
       </c>
       <c r="K146" s="11" t="s"/>
-      <c r="L146" s="95" t="s"/>
+      <c r="L146" s="98" t="s"/>
       <c r="M146" s="31" t="s">
         <v>50</v>
       </c>
@@ -7618,7 +7654,7 @@
         <f>=IF(M146="是",D146-N146,0)</f>
         <v>0</v>
       </c>
-      <c r="S146" s="92" t="s"/>
+      <c r="S146" s="95" t="s"/>
       <c r="U146" s="35" t="s"/>
     </row>
     <row r="147" spans="1:21">
@@ -7646,7 +7682,7 @@
         <v>45</v>
       </c>
       <c r="K147" s="11" t="s"/>
-      <c r="L147" s="95" t="s"/>
+      <c r="L147" s="98" t="s"/>
       <c r="M147" s="31" t="s">
         <v>50</v>
       </c>
@@ -7657,7 +7693,7 @@
         <f>=IF(M147="是",D147-N147,0)</f>
         <v>0</v>
       </c>
-      <c r="S147" s="92" t="s"/>
+      <c r="S147" s="95" t="s"/>
       <c r="U147" s="35" t="s"/>
     </row>
     <row r="148" spans="1:21">
@@ -7685,7 +7721,7 @@
         <v>45</v>
       </c>
       <c r="K148" s="11" t="s"/>
-      <c r="L148" s="95" t="s"/>
+      <c r="L148" s="98" t="s"/>
       <c r="M148" s="31" t="s">
         <v>50</v>
       </c>
@@ -7696,7 +7732,7 @@
         <f>=IF(M148="是",D148-N148,0)</f>
         <v>0</v>
       </c>
-      <c r="S148" s="92" t="s"/>
+      <c r="S148" s="95" t="s"/>
       <c r="U148" s="35" t="s"/>
     </row>
     <row r="149" spans="1:21">
@@ -7724,7 +7760,7 @@
         <v>45</v>
       </c>
       <c r="K149" s="11" t="s"/>
-      <c r="L149" s="95" t="s"/>
+      <c r="L149" s="98" t="s"/>
       <c r="M149" s="31" t="s">
         <v>50</v>
       </c>
@@ -7735,7 +7771,7 @@
         <f>=IF(M149="是",D149-N149,0)</f>
         <v>0</v>
       </c>
-      <c r="S149" s="92" t="s"/>
+      <c r="S149" s="95" t="s"/>
       <c r="U149" s="35" t="s"/>
     </row>
     <row r="150" spans="1:21">
@@ -7763,7 +7799,7 @@
         <v>45</v>
       </c>
       <c r="K150" s="11" t="s"/>
-      <c r="L150" s="95" t="s"/>
+      <c r="L150" s="98" t="s"/>
       <c r="M150" s="31" t="s">
         <v>50</v>
       </c>
@@ -7774,7 +7810,7 @@
         <f>=IF(M150="是",D150-N150,0)</f>
         <v>0</v>
       </c>
-      <c r="S150" s="92" t="s"/>
+      <c r="S150" s="95" t="s"/>
       <c r="U150" s="35" t="s"/>
     </row>
     <row r="151" spans="1:21">
@@ -7802,7 +7838,7 @@
         <v>45</v>
       </c>
       <c r="K151" s="11" t="s"/>
-      <c r="L151" s="95" t="s"/>
+      <c r="L151" s="98" t="s"/>
       <c r="M151" s="31" t="s">
         <v>50</v>
       </c>
@@ -7813,7 +7849,7 @@
         <f>=IF(M151="是",D151-N151,0)</f>
         <v>0</v>
       </c>
-      <c r="S151" s="92" t="s"/>
+      <c r="S151" s="95" t="s"/>
       <c r="U151" s="35" t="s"/>
     </row>
     <row r="152" spans="1:21">
@@ -7841,7 +7877,7 @@
         <v>45</v>
       </c>
       <c r="K152" s="11" t="s"/>
-      <c r="L152" s="95" t="s"/>
+      <c r="L152" s="98" t="s"/>
       <c r="M152" s="31" t="s">
         <v>50</v>
       </c>
@@ -7852,7 +7888,7 @@
         <f>=IF(M152="是",D152-N152,0)</f>
         <v>0</v>
       </c>
-      <c r="S152" s="92" t="s"/>
+      <c r="S152" s="95" t="s"/>
       <c r="U152" s="35" t="s"/>
     </row>
     <row r="153" spans="1:21">
@@ -7880,7 +7916,7 @@
         <v>45</v>
       </c>
       <c r="K153" s="11" t="s"/>
-      <c r="L153" s="95" t="s"/>
+      <c r="L153" s="98" t="s"/>
       <c r="M153" s="31" t="s">
         <v>50</v>
       </c>
@@ -7891,7 +7927,7 @@
         <f>=IF(M153="是",D153-N153,0)</f>
         <v>0</v>
       </c>
-      <c r="S153" s="92" t="s"/>
+      <c r="S153" s="95" t="s"/>
       <c r="U153" s="35" t="s"/>
     </row>
     <row r="154" spans="1:21">
@@ -7919,7 +7955,7 @@
         <v>45</v>
       </c>
       <c r="K154" s="11" t="s"/>
-      <c r="L154" s="95" t="s"/>
+      <c r="L154" s="98" t="s"/>
       <c r="M154" s="31" t="s">
         <v>50</v>
       </c>
@@ -7930,7 +7966,7 @@
         <f>=IF(M154="是",D154-N154,0)</f>
         <v>0</v>
       </c>
-      <c r="S154" s="92" t="s"/>
+      <c r="S154" s="95" t="s"/>
       <c r="U154" s="35" t="s"/>
     </row>
     <row r="155" spans="1:21">
@@ -7958,7 +7994,7 @@
         <v>45</v>
       </c>
       <c r="K155" s="11" t="s"/>
-      <c r="L155" s="95" t="s"/>
+      <c r="L155" s="98" t="s"/>
       <c r="M155" s="31" t="s">
         <v>50</v>
       </c>
@@ -7969,7 +8005,7 @@
         <f>=IF(M155="是",D155-N155,0)</f>
         <v>0</v>
       </c>
-      <c r="S155" s="92" t="s"/>
+      <c r="S155" s="95" t="s"/>
       <c r="U155" s="35" t="s"/>
     </row>
     <row r="156" spans="1:21">
@@ -7997,7 +8033,7 @@
         <v>45</v>
       </c>
       <c r="K156" s="11" t="s"/>
-      <c r="L156" s="95" t="s"/>
+      <c r="L156" s="98" t="s"/>
       <c r="M156" s="31" t="s">
         <v>50</v>
       </c>
@@ -8008,7 +8044,7 @@
         <f>=IF(M156="是",D156-N156,0)</f>
         <v>0</v>
       </c>
-      <c r="S156" s="92" t="s"/>
+      <c r="S156" s="95" t="s"/>
       <c r="U156" s="35" t="s"/>
     </row>
     <row r="157" spans="1:21">
@@ -8036,7 +8072,7 @@
         <v>45</v>
       </c>
       <c r="K157" s="11" t="s"/>
-      <c r="L157" s="95" t="s"/>
+      <c r="L157" s="98" t="s"/>
       <c r="M157" s="31" t="s">
         <v>50</v>
       </c>
@@ -8047,7 +8083,7 @@
         <f>=IF(M157="是",D157-N157,0)</f>
         <v>0</v>
       </c>
-      <c r="S157" s="92" t="s"/>
+      <c r="S157" s="95" t="s"/>
       <c r="U157" s="35" t="s"/>
     </row>
     <row r="158" spans="1:21">
@@ -8075,7 +8111,7 @@
         <v>45</v>
       </c>
       <c r="K158" s="11" t="s"/>
-      <c r="L158" s="95" t="s"/>
+      <c r="L158" s="98" t="s"/>
       <c r="M158" s="31" t="s">
         <v>50</v>
       </c>
@@ -8086,7 +8122,7 @@
         <f>=IF(M158="是",D158-N158,0)</f>
         <v>0</v>
       </c>
-      <c r="S158" s="92" t="s"/>
+      <c r="S158" s="95" t="s"/>
       <c r="U158" s="35" t="s"/>
     </row>
     <row r="159" spans="1:21">
@@ -8114,7 +8150,7 @@
         <v>45</v>
       </c>
       <c r="K159" s="11" t="s"/>
-      <c r="L159" s="95" t="s"/>
+      <c r="L159" s="98" t="s"/>
       <c r="M159" s="31" t="s">
         <v>50</v>
       </c>
@@ -8125,7 +8161,7 @@
         <f>=IF(M159="是",D159-N159,0)</f>
         <v>0</v>
       </c>
-      <c r="S159" s="92" t="s"/>
+      <c r="S159" s="95" t="s"/>
       <c r="U159" s="35" t="s"/>
     </row>
     <row r="160" spans="1:21">
@@ -8153,7 +8189,7 @@
         <v>45</v>
       </c>
       <c r="K160" s="11" t="s"/>
-      <c r="L160" s="95" t="s"/>
+      <c r="L160" s="98" t="s"/>
       <c r="M160" s="31" t="s">
         <v>50</v>
       </c>
@@ -8164,7 +8200,7 @@
         <f>=IF(M160="是",D160-N160,0)</f>
         <v>0</v>
       </c>
-      <c r="S160" s="92" t="s"/>
+      <c r="S160" s="95" t="s"/>
       <c r="U160" s="35" t="s"/>
     </row>
     <row r="161" spans="1:21">
@@ -8192,7 +8228,7 @@
         <v>45</v>
       </c>
       <c r="K161" s="11" t="s"/>
-      <c r="L161" s="95" t="s"/>
+      <c r="L161" s="98" t="s"/>
       <c r="M161" s="31" t="s">
         <v>50</v>
       </c>
@@ -8203,7 +8239,7 @@
         <f>=IF(M161="是",D161-N161,0)</f>
         <v>0</v>
       </c>
-      <c r="S161" s="92" t="s"/>
+      <c r="S161" s="95" t="s"/>
       <c r="U161" s="35" t="s"/>
     </row>
     <row r="162" spans="1:21">
@@ -8231,7 +8267,7 @@
         <v>45</v>
       </c>
       <c r="K162" s="11" t="s"/>
-      <c r="L162" s="95" t="s"/>
+      <c r="L162" s="98" t="s"/>
       <c r="M162" s="31" t="s">
         <v>50</v>
       </c>
@@ -8242,7 +8278,7 @@
         <f>=IF(M162="是",D162-N162,0)</f>
         <v>0</v>
       </c>
-      <c r="S162" s="92" t="s"/>
+      <c r="S162" s="95" t="s"/>
       <c r="U162" s="35" t="s"/>
     </row>
     <row r="163" spans="1:21">
@@ -8270,7 +8306,7 @@
         <v>45</v>
       </c>
       <c r="K163" s="11" t="s"/>
-      <c r="L163" s="95" t="s"/>
+      <c r="L163" s="98" t="s"/>
       <c r="M163" s="31" t="s">
         <v>50</v>
       </c>
@@ -8281,7 +8317,7 @@
         <f>=IF(M163="是",D163-N163,0)</f>
         <v>0</v>
       </c>
-      <c r="S163" s="92" t="s"/>
+      <c r="S163" s="95" t="s"/>
       <c r="U163" s="35" t="s"/>
     </row>
     <row r="164" spans="1:21">
@@ -8309,7 +8345,7 @@
         <v>45</v>
       </c>
       <c r="K164" s="11" t="s"/>
-      <c r="L164" s="95" t="s"/>
+      <c r="L164" s="98" t="s"/>
       <c r="M164" s="31" t="s">
         <v>50</v>
       </c>
@@ -8320,7 +8356,7 @@
         <f>=IF(M164="是",D164-N164,0)</f>
         <v>0</v>
       </c>
-      <c r="S164" s="92" t="s"/>
+      <c r="S164" s="95" t="s"/>
       <c r="U164" s="35" t="s"/>
     </row>
     <row r="165" spans="1:21">
@@ -8348,7 +8384,7 @@
         <v>45</v>
       </c>
       <c r="K165" s="11" t="s"/>
-      <c r="L165" s="95" t="s"/>
+      <c r="L165" s="98" t="s"/>
       <c r="M165" s="31" t="s">
         <v>50</v>
       </c>
@@ -8359,7 +8395,7 @@
         <f>=IF(M165="是",D165-N165,0)</f>
         <v>0</v>
       </c>
-      <c r="S165" s="92" t="s"/>
+      <c r="S165" s="95" t="s"/>
       <c r="U165" s="35" t="s"/>
     </row>
     <row r="166" spans="1:21">
@@ -8387,7 +8423,7 @@
         <v>45</v>
       </c>
       <c r="K166" s="11" t="s"/>
-      <c r="L166" s="95" t="s"/>
+      <c r="L166" s="98" t="s"/>
       <c r="M166" s="31" t="s">
         <v>50</v>
       </c>
@@ -8398,7 +8434,7 @@
         <f>=IF(M166="是",D166-N166,0)</f>
         <v>0</v>
       </c>
-      <c r="S166" s="92" t="s"/>
+      <c r="S166" s="95" t="s"/>
       <c r="U166" s="35" t="s"/>
     </row>
     <row r="167" spans="1:21">
@@ -8426,7 +8462,7 @@
         <v>45</v>
       </c>
       <c r="K167" s="11" t="s"/>
-      <c r="L167" s="95" t="s"/>
+      <c r="L167" s="98" t="s"/>
       <c r="M167" s="31" t="s">
         <v>50</v>
       </c>
@@ -8437,7 +8473,7 @@
         <f>=IF(M167="是",D167-N167,0)</f>
         <v>0</v>
       </c>
-      <c r="S167" s="92" t="s"/>
+      <c r="S167" s="95" t="s"/>
       <c r="U167" s="35" t="s"/>
     </row>
     <row r="168" spans="1:21">
@@ -8465,7 +8501,7 @@
         <v>45</v>
       </c>
       <c r="K168" s="11" t="s"/>
-      <c r="L168" s="95" t="s"/>
+      <c r="L168" s="98" t="s"/>
       <c r="M168" s="31" t="s">
         <v>50</v>
       </c>
@@ -8476,7 +8512,7 @@
         <f>=IF(M168="是",D168-N168,0)</f>
         <v>0</v>
       </c>
-      <c r="S168" s="92" t="s"/>
+      <c r="S168" s="95" t="s"/>
       <c r="U168" s="35" t="s"/>
     </row>
     <row r="169" spans="1:21">
@@ -8504,7 +8540,7 @@
         <v>45</v>
       </c>
       <c r="K169" s="11" t="s"/>
-      <c r="L169" s="95" t="s"/>
+      <c r="L169" s="98" t="s"/>
       <c r="M169" s="31" t="s">
         <v>50</v>
       </c>
@@ -8515,7 +8551,7 @@
         <f>=IF(M169="是",D169-N169,0)</f>
         <v>0</v>
       </c>
-      <c r="S169" s="92" t="s"/>
+      <c r="S169" s="95" t="s"/>
       <c r="U169" s="35" t="s"/>
     </row>
     <row r="170" spans="1:21">
@@ -8543,7 +8579,7 @@
         <v>45</v>
       </c>
       <c r="K170" s="11" t="s"/>
-      <c r="L170" s="95" t="s"/>
+      <c r="L170" s="98" t="s"/>
       <c r="M170" s="31" t="s">
         <v>50</v>
       </c>
@@ -8554,7 +8590,7 @@
         <f>=IF(M170="是",D170-N170,0)</f>
         <v>0</v>
       </c>
-      <c r="S170" s="92" t="s"/>
+      <c r="S170" s="95" t="s"/>
       <c r="U170" s="35" t="s"/>
     </row>
     <row r="171" spans="1:21">
@@ -8582,7 +8618,7 @@
         <v>45</v>
       </c>
       <c r="K171" s="11" t="s"/>
-      <c r="L171" s="95" t="s"/>
+      <c r="L171" s="98" t="s"/>
       <c r="M171" s="31" t="s">
         <v>50</v>
       </c>
@@ -8593,7 +8629,7 @@
         <f>=IF(M171="是",D171-N171,0)</f>
         <v>0</v>
       </c>
-      <c r="S171" s="92" t="s"/>
+      <c r="S171" s="95" t="s"/>
       <c r="U171" s="35" t="s"/>
     </row>
     <row r="172" spans="1:21">
@@ -8621,7 +8657,7 @@
         <v>45</v>
       </c>
       <c r="K172" s="11" t="s"/>
-      <c r="L172" s="95" t="s"/>
+      <c r="L172" s="98" t="s"/>
       <c r="M172" s="31" t="s">
         <v>50</v>
       </c>
@@ -8632,7 +8668,7 @@
         <f>=IF(M172="是",D172-N172,0)</f>
         <v>0</v>
       </c>
-      <c r="S172" s="92" t="s"/>
+      <c r="S172" s="95" t="s"/>
       <c r="U172" s="35" t="s"/>
     </row>
     <row r="173" spans="1:21">
@@ -8660,7 +8696,7 @@
         <v>45</v>
       </c>
       <c r="K173" s="11" t="s"/>
-      <c r="L173" s="95" t="s"/>
+      <c r="L173" s="98" t="s"/>
       <c r="M173" s="31" t="s">
         <v>50</v>
       </c>
@@ -8671,7 +8707,7 @@
         <f>=IF(M173="是",D173-N173,0)</f>
         <v>0</v>
       </c>
-      <c r="S173" s="92" t="s"/>
+      <c r="S173" s="95" t="s"/>
       <c r="U173" s="35" t="s"/>
     </row>
     <row r="174" spans="1:21">
@@ -8699,7 +8735,7 @@
         <v>45</v>
       </c>
       <c r="K174" s="11" t="s"/>
-      <c r="L174" s="95" t="s"/>
+      <c r="L174" s="98" t="s"/>
       <c r="M174" s="31" t="s">
         <v>50</v>
       </c>
@@ -8710,7 +8746,7 @@
         <f>=IF(M174="是",D174-N174,0)</f>
         <v>0</v>
       </c>
-      <c r="S174" s="92" t="s"/>
+      <c r="S174" s="95" t="s"/>
       <c r="U174" s="35" t="s"/>
     </row>
     <row r="175" spans="1:21">
@@ -8738,7 +8774,7 @@
         <v>45</v>
       </c>
       <c r="K175" s="11" t="s"/>
-      <c r="L175" s="95" t="s"/>
+      <c r="L175" s="98" t="s"/>
       <c r="M175" s="31" t="s">
         <v>50</v>
       </c>
@@ -8749,7 +8785,7 @@
         <f>=IF(M175="是",D175-N175,0)</f>
         <v>0</v>
       </c>
-      <c r="S175" s="92" t="s"/>
+      <c r="S175" s="95" t="s"/>
       <c r="U175" s="35" t="s"/>
     </row>
     <row r="176" spans="1:21">
@@ -8777,7 +8813,7 @@
         <v>45</v>
       </c>
       <c r="K176" s="11" t="s"/>
-      <c r="L176" s="95" t="s"/>
+      <c r="L176" s="98" t="s"/>
       <c r="M176" s="31" t="s">
         <v>50</v>
       </c>
@@ -8788,7 +8824,7 @@
         <f>=IF(M176="是",D176-N176,0)</f>
         <v>0</v>
       </c>
-      <c r="S176" s="92" t="s"/>
+      <c r="S176" s="95" t="s"/>
       <c r="U176" s="35" t="s"/>
     </row>
     <row r="177" spans="1:21">
@@ -8816,7 +8852,7 @@
         <v>45</v>
       </c>
       <c r="K177" s="11" t="s"/>
-      <c r="L177" s="95" t="s"/>
+      <c r="L177" s="98" t="s"/>
       <c r="M177" s="31" t="s">
         <v>50</v>
       </c>
@@ -8827,7 +8863,7 @@
         <f>=IF(M177="是",D177-N177,0)</f>
         <v>0</v>
       </c>
-      <c r="S177" s="92" t="s"/>
+      <c r="S177" s="95" t="s"/>
       <c r="U177" s="35" t="s"/>
     </row>
     <row r="178" spans="1:21">
@@ -8855,7 +8891,7 @@
         <v>45</v>
       </c>
       <c r="K178" s="11" t="s"/>
-      <c r="L178" s="95" t="s"/>
+      <c r="L178" s="98" t="s"/>
       <c r="M178" s="31" t="s">
         <v>50</v>
       </c>
@@ -8866,7 +8902,7 @@
         <f>=IF(M178="是",D178-N178,0)</f>
         <v>0</v>
       </c>
-      <c r="S178" s="92" t="s"/>
+      <c r="S178" s="95" t="s"/>
       <c r="U178" s="35" t="s"/>
     </row>
     <row r="179" spans="1:21">
@@ -8894,7 +8930,7 @@
         <v>45</v>
       </c>
       <c r="K179" s="11" t="s"/>
-      <c r="L179" s="95" t="s"/>
+      <c r="L179" s="98" t="s"/>
       <c r="M179" s="31" t="s">
         <v>50</v>
       </c>
@@ -8905,7 +8941,7 @@
         <f>=IF(M179="是",D179-N179,0)</f>
         <v>0</v>
       </c>
-      <c r="S179" s="92" t="s"/>
+      <c r="S179" s="95" t="s"/>
       <c r="U179" s="35" t="s"/>
     </row>
     <row r="180" spans="1:21">
@@ -8933,7 +8969,7 @@
         <v>45</v>
       </c>
       <c r="K180" s="11" t="s"/>
-      <c r="L180" s="95" t="s"/>
+      <c r="L180" s="98" t="s"/>
       <c r="M180" s="31" t="s">
         <v>50</v>
       </c>
@@ -8944,7 +8980,7 @@
         <f>=IF(M180="是",D180-N180,0)</f>
         <v>0</v>
       </c>
-      <c r="S180" s="92" t="s"/>
+      <c r="S180" s="95" t="s"/>
       <c r="U180" s="35" t="s"/>
     </row>
     <row r="181" spans="1:21">
@@ -8972,7 +9008,7 @@
         <v>45</v>
       </c>
       <c r="K181" s="11" t="s"/>
-      <c r="L181" s="95" t="s"/>
+      <c r="L181" s="98" t="s"/>
       <c r="M181" s="31" t="s">
         <v>50</v>
       </c>
@@ -8983,7 +9019,7 @@
         <f>=IF(M181="是",D181-N181,0)</f>
         <v>0</v>
       </c>
-      <c r="S181" s="92" t="s"/>
+      <c r="S181" s="95" t="s"/>
       <c r="U181" s="35" t="s"/>
     </row>
     <row r="182" spans="1:21">
@@ -9011,7 +9047,7 @@
         <v>45</v>
       </c>
       <c r="K182" s="11" t="s"/>
-      <c r="L182" s="95" t="s"/>
+      <c r="L182" s="98" t="s"/>
       <c r="M182" s="31" t="s">
         <v>50</v>
       </c>
@@ -9022,7 +9058,7 @@
         <f>=IF(M182="是",D182-N182,0)</f>
         <v>0</v>
       </c>
-      <c r="S182" s="92" t="s"/>
+      <c r="S182" s="95" t="s"/>
       <c r="U182" s="35" t="s"/>
     </row>
     <row r="183" spans="1:21">
@@ -9050,7 +9086,7 @@
         <v>45</v>
       </c>
       <c r="K183" s="11" t="s"/>
-      <c r="L183" s="95" t="s"/>
+      <c r="L183" s="98" t="s"/>
       <c r="M183" s="31" t="s">
         <v>50</v>
       </c>
@@ -9061,7 +9097,7 @@
         <f>=IF(M183="是",D183-N183,0)</f>
         <v>0</v>
       </c>
-      <c r="S183" s="92" t="s"/>
+      <c r="S183" s="95" t="s"/>
       <c r="U183" s="35" t="s"/>
     </row>
     <row r="184" spans="1:21">
@@ -9089,7 +9125,7 @@
         <v>45</v>
       </c>
       <c r="K184" s="11" t="s"/>
-      <c r="L184" s="95" t="s"/>
+      <c r="L184" s="98" t="s"/>
       <c r="M184" s="31" t="s">
         <v>50</v>
       </c>
@@ -9100,7 +9136,7 @@
         <f>=IF(M184="是",D184-N184,0)</f>
         <v>0</v>
       </c>
-      <c r="S184" s="92" t="s"/>
+      <c r="S184" s="95" t="s"/>
       <c r="U184" s="35" t="s"/>
     </row>
     <row r="185" spans="1:21">
@@ -9128,7 +9164,7 @@
         <v>45</v>
       </c>
       <c r="K185" s="11" t="s"/>
-      <c r="L185" s="95" t="s"/>
+      <c r="L185" s="98" t="s"/>
       <c r="M185" s="31" t="s">
         <v>50</v>
       </c>
@@ -9139,7 +9175,7 @@
         <f>=IF(M185="是",D185-N185,0)</f>
         <v>0</v>
       </c>
-      <c r="S185" s="92" t="s"/>
+      <c r="S185" s="95" t="s"/>
       <c r="U185" s="35" t="s"/>
     </row>
     <row r="186" spans="1:21">
@@ -9167,7 +9203,7 @@
         <v>45</v>
       </c>
       <c r="K186" s="11" t="s"/>
-      <c r="L186" s="95" t="s"/>
+      <c r="L186" s="98" t="s"/>
       <c r="M186" s="31" t="s">
         <v>50</v>
       </c>
@@ -9178,7 +9214,7 @@
         <f>=IF(M186="是",D186-N186,0)</f>
         <v>0</v>
       </c>
-      <c r="S186" s="92" t="s"/>
+      <c r="S186" s="95" t="s"/>
       <c r="U186" s="35" t="s"/>
     </row>
     <row r="187" spans="1:21">
@@ -9206,7 +9242,7 @@
         <v>45</v>
       </c>
       <c r="K187" s="11" t="s"/>
-      <c r="L187" s="95" t="s"/>
+      <c r="L187" s="98" t="s"/>
       <c r="M187" s="31" t="s">
         <v>50</v>
       </c>
@@ -9217,7 +9253,7 @@
         <f>=IF(M187="是",D187-N187,0)</f>
         <v>0</v>
       </c>
-      <c r="S187" s="92" t="s"/>
+      <c r="S187" s="95" t="s"/>
       <c r="U187" s="35" t="s"/>
     </row>
     <row r="188" spans="1:21">
@@ -9245,7 +9281,7 @@
         <v>45</v>
       </c>
       <c r="K188" s="11" t="s"/>
-      <c r="L188" s="95" t="s"/>
+      <c r="L188" s="98" t="s"/>
       <c r="M188" s="31" t="s">
         <v>50</v>
       </c>
@@ -9256,7 +9292,7 @@
         <f>=IF(M188="是",D188-N188,0)</f>
         <v>0</v>
       </c>
-      <c r="S188" s="92" t="s"/>
+      <c r="S188" s="95" t="s"/>
       <c r="U188" s="35" t="s"/>
     </row>
     <row r="189" spans="1:21">
@@ -9284,7 +9320,7 @@
         <v>45</v>
       </c>
       <c r="K189" s="11" t="s"/>
-      <c r="L189" s="95" t="s"/>
+      <c r="L189" s="98" t="s"/>
       <c r="M189" s="31" t="s">
         <v>50</v>
       </c>
@@ -9295,7 +9331,7 @@
         <f>=IF(M189="是",D189-N189,0)</f>
         <v>0</v>
       </c>
-      <c r="S189" s="92" t="s"/>
+      <c r="S189" s="95" t="s"/>
       <c r="U189" s="35" t="s"/>
     </row>
     <row r="190" spans="1:21">
@@ -9323,7 +9359,7 @@
         <v>45</v>
       </c>
       <c r="K190" s="11" t="s"/>
-      <c r="L190" s="95" t="s"/>
+      <c r="L190" s="98" t="s"/>
       <c r="M190" s="31" t="s">
         <v>50</v>
       </c>
@@ -9334,7 +9370,7 @@
         <f>=IF(M190="是",D190-N190,0)</f>
         <v>0</v>
       </c>
-      <c r="S190" s="92" t="s"/>
+      <c r="S190" s="95" t="s"/>
       <c r="U190" s="35" t="s"/>
     </row>
     <row r="191" spans="1:21">
@@ -9362,7 +9398,7 @@
         <v>45</v>
       </c>
       <c r="K191" s="11" t="s"/>
-      <c r="L191" s="95" t="s"/>
+      <c r="L191" s="98" t="s"/>
       <c r="M191" s="31" t="s">
         <v>50</v>
       </c>
@@ -9373,7 +9409,7 @@
         <f>=IF(M191="是",D191-N191,0)</f>
         <v>0</v>
       </c>
-      <c r="S191" s="92" t="s"/>
+      <c r="S191" s="95" t="s"/>
       <c r="U191" s="35" t="s"/>
     </row>
     <row r="192" spans="1:21">
@@ -9401,7 +9437,7 @@
         <v>45</v>
       </c>
       <c r="K192" s="11" t="s"/>
-      <c r="L192" s="95" t="s"/>
+      <c r="L192" s="98" t="s"/>
       <c r="M192" s="31" t="s">
         <v>50</v>
       </c>
@@ -9412,7 +9448,7 @@
         <f>=IF(M192="是",D192-N192,0)</f>
         <v>0</v>
       </c>
-      <c r="S192" s="92" t="s"/>
+      <c r="S192" s="95" t="s"/>
       <c r="U192" s="35" t="s"/>
     </row>
     <row r="193" spans="1:21">
@@ -9440,7 +9476,7 @@
         <v>45</v>
       </c>
       <c r="K193" s="11" t="s"/>
-      <c r="L193" s="95" t="s"/>
+      <c r="L193" s="98" t="s"/>
       <c r="M193" s="31" t="s">
         <v>50</v>
       </c>
@@ -9451,7 +9487,7 @@
         <f>=IF(M193="是",D193-N193,0)</f>
         <v>0</v>
       </c>
-      <c r="S193" s="92" t="s"/>
+      <c r="S193" s="95" t="s"/>
       <c r="U193" s="35" t="s"/>
     </row>
     <row r="194" spans="1:21">
@@ -9479,7 +9515,7 @@
         <v>45</v>
       </c>
       <c r="K194" s="11" t="s"/>
-      <c r="L194" s="95" t="s"/>
+      <c r="L194" s="98" t="s"/>
       <c r="M194" s="31" t="s">
         <v>50</v>
       </c>
@@ -9490,7 +9526,7 @@
         <f>=IF(M194="是",D194-N194,0)</f>
         <v>0</v>
       </c>
-      <c r="S194" s="92" t="s"/>
+      <c r="S194" s="95" t="s"/>
       <c r="U194" s="35" t="s"/>
     </row>
     <row r="195" spans="1:21">
@@ -9518,7 +9554,7 @@
         <v>45</v>
       </c>
       <c r="K195" s="11" t="s"/>
-      <c r="L195" s="95" t="s"/>
+      <c r="L195" s="98" t="s"/>
       <c r="M195" s="31" t="s">
         <v>50</v>
       </c>
@@ -9529,7 +9565,7 @@
         <f>=IF(M195="是",D195-N195,0)</f>
         <v>0</v>
       </c>
-      <c r="S195" s="92" t="s"/>
+      <c r="S195" s="95" t="s"/>
       <c r="U195" s="35" t="s"/>
     </row>
     <row r="196" spans="1:21">
@@ -9557,7 +9593,7 @@
         <v>45</v>
       </c>
       <c r="K196" s="11" t="s"/>
-      <c r="L196" s="95" t="s"/>
+      <c r="L196" s="98" t="s"/>
       <c r="M196" s="31" t="s">
         <v>50</v>
       </c>
@@ -9568,7 +9604,7 @@
         <f>=IF(M196="是",D196-N196,0)</f>
         <v>0</v>
       </c>
-      <c r="S196" s="92" t="s"/>
+      <c r="S196" s="95" t="s"/>
       <c r="U196" s="35" t="s"/>
     </row>
     <row r="197" spans="1:21">
@@ -9596,7 +9632,7 @@
         <v>45</v>
       </c>
       <c r="K197" s="11" t="s"/>
-      <c r="L197" s="95" t="s"/>
+      <c r="L197" s="98" t="s"/>
       <c r="M197" s="31" t="s">
         <v>50</v>
       </c>
@@ -9607,7 +9643,7 @@
         <f>=IF(M197="是",D197-N197,0)</f>
         <v>0</v>
       </c>
-      <c r="S197" s="92" t="s"/>
+      <c r="S197" s="95" t="s"/>
       <c r="U197" s="35" t="s"/>
     </row>
     <row r="198" spans="1:21">
@@ -9635,7 +9671,7 @@
         <v>45</v>
       </c>
       <c r="K198" s="11" t="s"/>
-      <c r="L198" s="95" t="s"/>
+      <c r="L198" s="98" t="s"/>
       <c r="M198" s="31" t="s">
         <v>50</v>
       </c>
@@ -9646,7 +9682,7 @@
         <f>=IF(M198="是",D198-N198,0)</f>
         <v>0</v>
       </c>
-      <c r="S198" s="92" t="s"/>
+      <c r="S198" s="95" t="s"/>
       <c r="U198" s="35" t="s"/>
     </row>
     <row r="199" spans="1:21">
@@ -9674,7 +9710,7 @@
         <v>45</v>
       </c>
       <c r="K199" s="11" t="s"/>
-      <c r="L199" s="95" t="s"/>
+      <c r="L199" s="98" t="s"/>
       <c r="M199" s="31" t="s">
         <v>50</v>
       </c>
@@ -9685,7 +9721,7 @@
         <f>=IF(M199="是",D199-N199,0)</f>
         <v>0</v>
       </c>
-      <c r="S199" s="92" t="s"/>
+      <c r="S199" s="95" t="s"/>
       <c r="U199" s="35" t="s"/>
     </row>
     <row r="200" spans="1:21">
@@ -9713,7 +9749,7 @@
         <v>45</v>
       </c>
       <c r="K200" s="11" t="s"/>
-      <c r="L200" s="95" t="s"/>
+      <c r="L200" s="98" t="s"/>
       <c r="M200" s="31" t="s">
         <v>50</v>
       </c>
@@ -9724,23 +9760,23 @@
         <f>=IF(M200="是",D200-N200,0)</f>
         <v>0</v>
       </c>
-      <c r="S200" s="92" t="s"/>
+      <c r="S200" s="95" t="s"/>
       <c r="U200" s="35" t="s"/>
     </row>
     <row r="201" spans="3:21">
       <c r="C201" s="29" t="s"/>
-      <c r="M201" s="96" t="s"/>
-      <c r="N201" s="96" t="s"/>
-      <c r="O201" s="97" t="s"/>
-      <c r="S201" s="92" t="s"/>
+      <c r="M201" s="99" t="s"/>
+      <c r="N201" s="99" t="s"/>
+      <c r="O201" s="100" t="s"/>
+      <c r="S201" s="95" t="s"/>
       <c r="U201" s="35" t="s"/>
     </row>
     <row r="202" spans="3:21">
       <c r="C202" s="29" t="s"/>
-      <c r="M202" s="96" t="s"/>
-      <c r="N202" s="96" t="s"/>
-      <c r="O202" s="97" t="s"/>
-      <c r="S202" s="92" t="s"/>
+      <c r="M202" s="99" t="s"/>
+      <c r="N202" s="99" t="s"/>
+      <c r="O202" s="100" t="s"/>
+      <c r="S202" s="95" t="s"/>
       <c r="U202" s="35" t="s"/>
     </row>
   </sheetData>
@@ -9750,7 +9786,7 @@
   </mergeCells>
   <dataValidations>
     <dataValidation type="list" errorStyle="stop" allowBlank="true" showDropDown="false" showInputMessage="true" showErrorMessage="true" prompt="" sqref="C2:C1048576">
-      <formula1>"Nexys-Video,PYNQ-Z2,ACZ7015,ZCU104,Zedboard,ACX750,MLK-KU060,VD100,Alveo-U45N,Alveo-U55C,KV260,KU5P,Boolean,AXP391,EQ6HL45,11EG,"</formula1>
+      <formula1>"Nexys-Video,PYNQ-Z2,ACZ7015,ZCU104,Zedboard,ACX750,MLK-KU060,VD100,Alveo-U45N,Alveo-U55C,KV260,KU5P,Boolean,AXP391,EQ6HL45,11EG,ZU19EG,"</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="stop" allowBlank="true" showDropDown="false" showInputMessage="true" showErrorMessage="true" prompt="" sqref="H2:H200">
       <formula1>"叶秉泽,"</formula1>

</xml_diff>

<commit_message>
Board File Update on 11.10
</commit_message>
<xml_diff>
--- a/DeviceManagement/HIQC板卡统计及出借情况.xlsx
+++ b/DeviceManagement/HIQC板卡统计及出借情况.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
   <si>
     <t/>
   </si>
@@ -248,6 +248,12 @@
   </si>
   <si>
     <t>陈凯</t>
+  </si>
+  <si>
+    <t>沈阳</t>
+  </si>
+  <si>
+    <t>11EG</t>
   </si>
   <si>
     <r>
@@ -1437,7 +1443,7 @@
         <v>1</v>
       </c>
       <c r="P2" s="23" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="Q2" s="24" t="s"/>
       <c r="R2" s="25" t="s"/>
@@ -2013,7 +2019,7 @@
         <v>8</v>
       </c>
       <c r="Q11" s="50" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="R11" s="51">
         <f>=SUMIF($C$2:$C$200,"VD100",E2:E200)</f>
@@ -2210,14 +2216,14 @@
       </c>
       <c r="R14" s="61">
         <f>=SUMIF($C$2:$C$200,"KV260",E2:E200)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S14" s="61">
         <v>4</v>
       </c>
       <c r="T14" s="62">
         <f>=S14-R14</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U14" s="63" t="s"/>
     </row>
@@ -2520,14 +2526,14 @@
       </c>
       <c r="R19" s="78">
         <f>=SUMIF($C$2:$C$200,"11EG",E2:E200)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S19" s="79">
         <v>4</v>
       </c>
       <c r="T19" s="80">
         <f>=S19-R19</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U19" s="76" t="s"/>
       <c r="V19" s="58" t="s"/>
@@ -3231,16 +3237,22 @@
       <c r="A34" s="14">
         <v>32</v>
       </c>
-      <c r="B34" s="10" t="s"/>
-      <c r="C34" s="29" t="s"/>
+      <c r="B34" s="86">
+        <v>45971</v>
+      </c>
+      <c r="C34" s="29" t="s">
+        <v>51</v>
+      </c>
       <c r="D34" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E34" s="14">
         <f>=D34-O34</f>
-        <v>0</v>
-      </c>
-      <c r="F34" s="14" t="s"/>
+        <v>1</v>
+      </c>
+      <c r="F34" s="14" t="s">
+        <v>78</v>
+      </c>
       <c r="G34" s="10" t="s"/>
       <c r="H34" s="29" t="s">
         <v>21</v>
@@ -3272,16 +3284,22 @@
       <c r="A35" s="14">
         <v>33</v>
       </c>
-      <c r="B35" s="10" t="s"/>
-      <c r="C35" s="29" t="s"/>
+      <c r="B35" s="86">
+        <v>45971</v>
+      </c>
+      <c r="C35" s="29" t="s">
+        <v>79</v>
+      </c>
       <c r="D35" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E35" s="14">
         <f>=D35-O35</f>
-        <v>0</v>
-      </c>
-      <c r="F35" s="14" t="s"/>
+        <v>1</v>
+      </c>
+      <c r="F35" s="14" t="s">
+        <v>78</v>
+      </c>
       <c r="G35" s="10" t="s"/>
       <c r="H35" s="29" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Board File Update on 11.19
</commit_message>
<xml_diff>
--- a/DeviceManagement/HIQC板卡统计及出借情况.xlsx
+++ b/DeviceManagement/HIQC板卡统计及出借情况.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
   <si>
     <t/>
   </si>
@@ -254,6 +254,9 @@
   </si>
   <si>
     <t>11EG</t>
+  </si>
+  <si>
+    <t>沈如祺</t>
   </si>
   <si>
     <r>
@@ -1443,7 +1446,7 @@
         <v>1</v>
       </c>
       <c r="P2" s="23" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="Q2" s="24" t="s"/>
       <c r="R2" s="25" t="s"/>
@@ -2019,7 +2022,7 @@
         <v>8</v>
       </c>
       <c r="Q11" s="50" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="R11" s="51">
         <f>=SUMIF($C$2:$C$200,"VD100",E2:E200)</f>
@@ -2216,14 +2219,14 @@
       </c>
       <c r="R14" s="61">
         <f>=SUMIF($C$2:$C$200,"KV260",E2:E200)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S14" s="61">
         <v>4</v>
       </c>
       <c r="T14" s="62">
         <f>=S14-R14</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U14" s="63" t="s"/>
     </row>
@@ -3332,16 +3335,22 @@
       <c r="A36" s="14">
         <v>34</v>
       </c>
-      <c r="B36" s="10" t="s"/>
-      <c r="C36" s="29" t="s"/>
+      <c r="B36" s="86">
+        <v>45980</v>
+      </c>
+      <c r="C36" s="29" t="s">
+        <v>51</v>
+      </c>
       <c r="D36" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E36" s="14">
         <f>=D36-O36</f>
-        <v>0</v>
-      </c>
-      <c r="F36" s="14" t="s"/>
+        <v>1</v>
+      </c>
+      <c r="F36" s="14" t="s">
+        <v>80</v>
+      </c>
       <c r="G36" s="10" t="s"/>
       <c r="H36" s="29" t="s">
         <v>21</v>

</xml_diff>